<commit_message>
Tweaking so that nosetests passes
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -399,9 +399,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -411,24 +411,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
     <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" t="n" s="1">
         <v>2.3</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" t="n" s="1">
         <v>2.4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -439,7 +439,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -454,9 +454,9 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -466,13 +466,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
     <col max="1" min="1" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Add named ranges to output for excel
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -7,10 +7,18 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="DisplayValues" r:id="rId1" sheetId="1"/>
     <sheet name="Lookups" r:id="rId2" sheetId="2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
+    <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$3</definedName>
+    <definedName name="dis_value_values">'DisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
+    <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
+    <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -399,7 +407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
@@ -411,41 +419,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s" s="1">
+      <c t="s" r="A1" s="1">
         <v>7</v>
       </c>
-      <c r="B1" t="n" s="1">
+      <c t="n" r="B1" s="1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n" s="1">
+      <c t="n" r="C1" s="1">
         <v>2.4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="n" s="1">
+      <c t="n" r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="n" s="1">
+      <c t="n" r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -454,7 +462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
@@ -466,63 +474,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+    <col min="6" max="6" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>6</v>
       </c>
-      <c r="G2" t="n">
+      <c t="n" r="G2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="F3" t="s">
+      <c t="s" r="F3">
         <v>5</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for end to end
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -407,36 +407,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="1" max="1" customWidth="true" width="9.1"/>
+    <col min="3" max="3" customWidth="true" width="9.1"/>
+    <col min="2" max="2" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c t="s" r="A1" s="1">
+    <row spans="1:3" r="1">
+      <c s="1" t="s" r="A1">
         <v>7</v>
       </c>
-      <c t="n" r="B1" s="1">
+      <c s="1" t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1" s="1">
+      <c s="1" t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c t="n" r="A2" s="1">
+    <row spans="1:3" r="2">
+      <c s="1" t="n" r="A2">
         <v>0</v>
       </c>
       <c t="n" r="B2">
@@ -446,8 +446,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c t="n" r="A3" s="1">
+    <row spans="1:3" r="3">
+      <c s="1" t="n" r="A3">
         <v>1</v>
       </c>
       <c t="n" r="B3">
@@ -462,28 +462,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="5" max="5" width="9.10"/>
     <col min="4" max="4" width="9.10"/>
-    <col min="5" max="5" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
     <col min="6" max="6" width="9.10"/>
-    <col min="7" max="7" width="9.10"/>
     <col min="1" max="1" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
     <col min="2" max="2" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row spans="1:7" r="1">
       <c t="s" r="A1">
         <v>2</v>
       </c>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row spans="1:7" r="2">
       <c t="s" r="A2">
         <v>4</v>
       </c>
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row spans="1:7" r="3">
       <c t="s" r="F3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Figure out why there are additional columns in display values
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -419,41 +419,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.1"/>
-    <col min="3" max="3" customWidth="true" width="9.1"/>
-    <col min="2" max="2" customWidth="true" width="9.1"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c s="1" t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c s="1" t="n" r="B1">
+      <c r="B1" s="1" t="n">
         <v>2.3</v>
       </c>
-      <c s="1" t="n" r="C1">
+      <c r="C1" s="1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c s="1" t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c s="1" t="n" r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -474,63 +474,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
-    <col min="7" max="7" width="9.10"/>
-    <col min="6" max="6" width="9.10"/>
-    <col min="1" max="1" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:7" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:7" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="G2">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:7" r="3">
-      <c t="s" r="F3">
+    <row r="3" spans="1:7">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add question code and result type to columns output
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -17,14 +17,14 @@
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$G$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Corps</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>question_code</t>
+  </si>
+  <si>
+    <t>result_type</t>
   </si>
   <si>
     <t>row_heading</t>
@@ -414,7 +420,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -426,7 +432,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>2.3</v>
@@ -466,10 +472,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,14 +487,18 @@
     <col max="5" min="5" width="9.10"/>
     <col max="6" min="6" width="9.10"/>
     <col max="7" min="7" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -502,13 +512,19 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -525,12 +541,36 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add default_menu_start named range
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -17,6 +17,7 @@
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
+    <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
     <definedName name="cuts_head">'Lookups'!$F$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -480,6 +481,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
     <col max="1" min="1" width="9.10"/>
     <col max="2" min="2" width="9.10"/>
     <col max="3" min="3" width="9.10"/>
@@ -487,10 +492,6 @@
     <col max="5" min="5" width="9.10"/>
     <col max="6" min="6" width="9.10"/>
     <col max="7" min="7" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
Use excel template specified in config
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -7,8 +7,9 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="DisplayValues" r:id="rId1" sheetId="1"/>
-    <sheet name="Lookups" r:id="rId2" sheetId="2"/>
+    <sheet name="ExistingData" r:id="rId1" sheetId="1"/>
+    <sheet name="DisplayValues" r:id="rId2" sheetId="2"/>
+    <sheet name="Lookups" r:id="rId3" sheetId="3"/>
   </sheets>
   <definedNames>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
@@ -65,20 +66,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,30 +91,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -414,7 +390,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -426,41 +418,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -468,8 +460,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -481,97 +473,97 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="8" min="8" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
+    <col min="8" max="8" width="9.10"/>
+    <col min="9" max="9" width="9.10"/>
+    <col min="10" max="10" width="9.10"/>
+    <col min="11" max="11" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+    <col min="6" max="6" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row spans="1:11" r="1">
+      <c t="s" r="A1">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row spans="1:11" r="2">
+      <c t="s" r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>6</v>
       </c>
-      <c r="G2" t="n">
+      <c t="n" r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c t="s" r="H2">
         <v>6</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="J2">
         <v>6</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="F3" t="s">
+    <row spans="1:11" r="3">
+      <c t="s" r="F3">
         <v>5</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="H3">
         <v>5</v>
       </c>
-      <c r="I3" t="n">
+      <c t="n" r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c t="s" r="J3">
         <v>5</v>
       </c>
-      <c r="K3" t="n">
+      <c t="n" r="K3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Overwrite existing named ranges
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -390,14 +390,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -406,53 +406,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
     <col min="1" width="9.1" customWidth="true" max="1"/>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c t="n" r="A2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c t="n" r="A3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -461,109 +461,109 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="9.10"/>
-    <col min="9" max="9" width="9.10"/>
-    <col min="10" max="10" width="9.10"/>
-    <col min="11" max="11" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
-    <col min="5" max="5" width="9.10"/>
-    <col min="6" max="6" width="9.10"/>
-    <col min="7" max="7" width="9.10"/>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
+    <col min="3" width="9.10" max="3"/>
+    <col min="2" width="9.10" max="2"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="7" width="9.10" max="7"/>
+    <col min="6" width="9.10" max="6"/>
+    <col min="5" width="9.10" max="5"/>
+    <col min="4" width="9.10" max="4"/>
+    <col min="11" width="9.10" max="11"/>
+    <col min="10" width="9.10" max="10"/>
+    <col min="9" width="9.10" max="9"/>
+    <col min="8" width="9.10" max="8"/>
   </cols>
   <sheetData>
     <row spans="1:11" r="1">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
     <row spans="1:11" r="2">
-      <c t="s" r="A2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="G2">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="H2">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="I2">
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="J2">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="K2">
+      <c r="K2" t="n">
         <v>0</v>
       </c>
     </row>
     <row spans="1:11" r="3">
-      <c t="s" r="F3">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c t="s" r="H3">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="I3">
+      <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c t="s" r="J3">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="K3">
+      <c r="K3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added migration script for moving to new db
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -18,6 +18,7 @@
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
+    <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
     <definedName name="cuts_head">'Lookups'!$F$1:$K$1</definedName>
   </definedNames>
@@ -418,41 +419,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col max="2" width="9.1" min="2" customWidth="true"/>
+    <col max="3" width="9.1" min="3" customWidth="true"/>
+    <col max="1" width="9.1" min="1" customWidth="true"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>9</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -473,97 +474,97 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" width="9.10" max="3"/>
-    <col min="2" width="9.10" max="2"/>
-    <col min="1" width="9.10" max="1"/>
-    <col min="7" width="9.10" max="7"/>
-    <col min="6" width="9.10" max="6"/>
-    <col min="5" width="9.10" max="5"/>
-    <col min="4" width="9.10" max="4"/>
-    <col min="11" width="9.10" max="11"/>
-    <col min="10" width="9.10" max="10"/>
-    <col min="9" width="9.10" max="9"/>
-    <col min="8" width="9.10" max="8"/>
+    <col max="6" width="9.10" min="6"/>
+    <col max="7" width="9.10" min="7"/>
+    <col max="4" width="9.10" min="4"/>
+    <col max="5" width="9.10" min="5"/>
+    <col max="2" width="9.10" min="2"/>
+    <col max="3" width="9.10" min="3"/>
+    <col max="1" width="9.10" min="1"/>
+    <col max="10" width="9.10" min="10"/>
+    <col max="11" width="9.10" min="11"/>
+    <col max="8" width="9.10" min="8"/>
+    <col max="9" width="9.10" min="9"/>
   </cols>
   <sheetData>
     <row spans="1:11" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>8</v>
       </c>
     </row>
     <row spans="1:11" r="2">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>6</v>
       </c>
-      <c r="G2" t="n">
+      <c t="n" r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c t="s" r="H2">
         <v>6</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="J2">
         <v>6</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="K2">
         <v>0</v>
       </c>
     </row>
     <row spans="1:11" r="3">
-      <c r="F3" t="s">
+      <c t="s" r="F3">
         <v>5</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="H3">
         <v>5</v>
       </c>
-      <c r="I3" t="n">
+      <c t="n" r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c t="s" r="J3">
         <v>5</v>
       </c>
-      <c r="K3" t="n">
+      <c t="n" r="K3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Export not included label with blank string by default
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
     <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$3</definedName>
-    <definedName name="dis_value_values">'DisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="disp_value_values">'DisplayValues'!$B$2:$C$3</definedName>
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Corps</t>
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Gender Not Used</t>
   </si>
   <si>
     <t>Grade</t>
@@ -393,12 +396,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -409,51 +412,51 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="2" width="9.1" min="2" customWidth="true"/>
-    <col max="3" width="9.1" min="3" customWidth="true"/>
-    <col max="1" width="9.1" min="1" customWidth="true"/>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
-        <v>9</v>
-      </c>
-      <c t="n" r="B1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -464,108 +467,116 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="6" width="9.10" min="6"/>
-    <col max="7" width="9.10" min="7"/>
-    <col max="4" width="9.10" min="4"/>
-    <col max="5" width="9.10" min="5"/>
-    <col max="2" width="9.10" min="2"/>
-    <col max="3" width="9.10" min="3"/>
-    <col max="1" width="9.10" min="1"/>
-    <col max="10" width="9.10" min="10"/>
-    <col max="11" width="9.10" min="11"/>
-    <col max="8" width="9.10" min="8"/>
-    <col max="9" width="9.10" min="9"/>
+    <col width="9.10" min="10" max="10"/>
+    <col width="9.10" min="11" max="11"/>
+    <col width="9.10" min="8" max="8"/>
+    <col width="9.10" min="9" max="9"/>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="6" max="6"/>
+    <col width="9.10" min="7" max="7"/>
+    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row spans="1:11" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="B1">
-        <v>10</v>
-      </c>
-      <c t="s" r="C1">
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="D1">
-        <v>4</v>
-      </c>
-      <c t="s" r="E1">
-        <v>0</v>
-      </c>
-      <c t="s" r="F1">
-        <v>1</v>
-      </c>
-      <c t="s" r="H1">
-        <v>7</v>
-      </c>
-      <c t="s" r="J1">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:11" r="2">
-      <c t="s" r="A2">
-        <v>4</v>
-      </c>
-      <c t="s" r="B2">
-        <v>10</v>
-      </c>
-      <c t="s" r="C2">
-        <v>4</v>
-      </c>
-      <c t="s" r="D2">
-        <v>0</v>
-      </c>
-      <c t="s" r="E2">
-        <v>3</v>
-      </c>
-      <c t="s" r="F2">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="G2">
-        <v>0</v>
-      </c>
-      <c t="s" r="H2">
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="I2">
-        <v>0</v>
-      </c>
-      <c t="s" r="J2">
-        <v>6</v>
-      </c>
-      <c t="n" r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:11" r="3">
-      <c t="s" r="F3">
-        <v>5</v>
-      </c>
-      <c t="n" r="G3">
-        <v>1</v>
-      </c>
-      <c t="s" r="H3">
-        <v>5</v>
-      </c>
-      <c t="n" r="I3">
-        <v>1</v>
-      </c>
-      <c t="s" r="J3">
-        <v>5</v>
-      </c>
-      <c t="n" r="K3">
-        <v>1</v>
+      <c r="G4" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Turn off not included label in dimension when desired
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -20,14 +20,14 @@
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
     <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$K$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Corps</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Gender Not Used</t>
+  </si>
+  <si>
+    <t>GenderB</t>
   </si>
   <si>
     <t>Grade</t>
@@ -422,14 +425,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="n">
         <v>2.3</v>
@@ -469,7 +472,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,31 +480,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="10" max="10"/>
-    <col width="9.10" min="11" max="11"/>
-    <col width="9.10" min="8" max="8"/>
-    <col width="9.10" min="9" max="9"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="6" max="6"/>
-    <col width="9.10" min="7" max="7"/>
-    <col width="9.10" min="4" max="4"/>
-    <col width="9.10" min="5" max="5"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -510,27 +515,30 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -539,41 +547,53 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" t="n">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="F4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Cleaning up workspace for additional work
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -399,12 +399,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -415,51 +415,51 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col width="9.1" max="3" min="3" customWidth="true"/>
+    <col width="9.1" max="2" min="2" customWidth="true"/>
+    <col width="9.1" max="1" min="1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>11</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -470,132 +470,132 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
+    <col width="9.10" max="3" min="3"/>
+    <col width="9.10" max="2" min="2"/>
+    <col width="9.10" max="1" min="1"/>
+    <col width="9.10" max="7" min="7"/>
+    <col width="9.10" max="6" min="6"/>
+    <col width="9.10" max="5" min="5"/>
+    <col width="9.10" max="4" min="4"/>
+    <col width="9.10" max="11" min="11"/>
+    <col width="9.10" max="10" min="10"/>
+    <col width="9.10" max="9" min="9"/>
+    <col width="9.10" max="8" min="8"/>
+    <col width="9.10" max="13" min="13"/>
+    <col width="9.10" max="12" min="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
+    <row spans="1:13" r="1">
+      <c t="s" r="A1">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+    <row spans="1:13" r="2">
+      <c t="s" r="A2">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c t="n" r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c t="s" r="H2">
         <v>8</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="I2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="J2">
         <v>8</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c t="s" r="L2">
         <v>8</v>
       </c>
-      <c r="M2" t="n">
+      <c t="n" r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="F3" t="s">
+    <row spans="1:13" r="3">
+      <c t="s" r="F3">
         <v>8</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="H3">
         <v>7</v>
       </c>
-      <c r="I3" t="n">
+      <c t="n" r="I3">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c t="s" r="J3">
         <v>7</v>
       </c>
-      <c r="K3" t="n">
+      <c t="n" r="K3">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c t="s" r="L3">
         <v>7</v>
       </c>
-      <c r="M3" t="n">
+      <c t="n" r="M3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="F4" t="s">
+    <row spans="1:13" r="4">
+      <c t="s" r="F4">
         <v>7</v>
       </c>
-      <c r="G4" t="n">
+      <c t="n" r="G4">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Bug SRS-25 so that it now checks that an entry exists for every combination of dimension values
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -397,14 +397,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,14 +413,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,36 +430,36 @@
     <col width="9.1" max="1" min="1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -468,134 +468,134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="3" min="3"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="1" min="1"/>
     <col width="9.10" max="7" min="7"/>
     <col width="9.10" max="6" min="6"/>
     <col width="9.10" max="5" min="5"/>
     <col width="9.10" max="4" min="4"/>
+    <col width="9.10" max="3" min="3"/>
+    <col width="9.10" max="2" min="2"/>
+    <col width="9.10" max="1" min="1"/>
+    <col width="9.10" max="13" min="13"/>
+    <col width="9.10" max="12" min="12"/>
     <col width="9.10" max="11" min="11"/>
     <col width="9.10" max="10" min="10"/>
     <col width="9.10" max="9" min="9"/>
     <col width="9.10" max="8" min="8"/>
-    <col width="9.10" max="13" min="13"/>
-    <col width="9.10" max="12" min="12"/>
   </cols>
   <sheetData>
-    <row spans="1:13" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="L1">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:13" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c t="n" r="G2">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="H2">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="I2">
+      <c r="I2" t="n">
         <v>1</v>
       </c>
-      <c t="s" r="J2">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="K2">
+      <c r="K2" t="n">
         <v>1</v>
       </c>
-      <c t="s" r="L2">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="M2">
+      <c r="M2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:13" r="3">
-      <c t="s" r="F3">
+    <row r="3" spans="1:13">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c t="s" r="H3">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="I3">
+      <c r="I3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="J3">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="K3">
+      <c r="K3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="L3">
+      <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="M3">
+      <c r="M3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:13" r="4">
-      <c t="s" r="F4">
+    <row r="4" spans="1:13">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="G4">
+      <c r="G4" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change "missing" label to "All [dimension] together"
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -399,7 +399,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
@@ -415,7 +415,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -425,12 +425,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="3" min="3" customWidth="true"/>
-    <col width="9.1" max="2" min="2" customWidth="true"/>
-    <col width="9.1" max="1" min="1" customWidth="true"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row spans="1:3" r="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -441,7 +441,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row spans="1:3" r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row spans="1:3" r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
@@ -470,7 +470,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -480,22 +480,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="7" min="7"/>
-    <col width="9.10" max="6" min="6"/>
-    <col width="9.10" max="5" min="5"/>
-    <col width="9.10" max="4" min="4"/>
-    <col width="9.10" max="3" min="3"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="1" min="1"/>
-    <col width="9.10" max="13" min="13"/>
-    <col width="9.10" max="12" min="12"/>
-    <col width="9.10" max="11" min="11"/>
-    <col width="9.10" max="10" min="10"/>
-    <col width="9.10" max="9" min="9"/>
-    <col width="9.10" max="8" min="8"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row spans="1:13" r="1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -524,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row spans="1:13" r="2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -541,16 +541,16 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
       </c>
       <c r="J2" t="s">
         <v>8</v>
@@ -565,18 +565,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row spans="1:13" r="3">
       <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
@@ -591,11 +591,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="F4" t="s">
+    <row spans="1:13" r="4">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add zero string label to dashboard
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -21,6 +21,7 @@
     <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
     <definedName name="cuts_head">'Lookups'!$F$1:$M$1</definedName>
+    <definedName name="zero_string">'Lookups'!$N$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
@@ -404,7 +405,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,46 +421,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="3" customWidth="true" width="9.1"/>
-    <col max="2" min="2" customWidth="true" width="9.1"/>
-    <col max="1" min="1" customWidth="true" width="9.1"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>11</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
+      <c t="n" r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -472,130 +473,134 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="13" min="13" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
+    <col max="12" width="9.10" min="12"/>
+    <col max="13" width="9.10" min="13"/>
+    <col max="14" width="9.10" min="14"/>
+    <col max="8" width="9.10" min="8"/>
+    <col max="9" width="9.10" min="9"/>
+    <col max="10" width="9.10" min="10"/>
+    <col max="11" width="9.10" min="11"/>
+    <col max="4" width="9.10" min="4"/>
+    <col max="5" width="9.10" min="5"/>
+    <col max="6" width="9.10" min="6"/>
+    <col max="7" width="9.10" min="7"/>
+    <col max="1" width="9.10" min="1"/>
+    <col max="2" width="9.10" min="2"/>
+    <col max="3" width="9.10" min="3"/>
   </cols>
   <sheetData>
-    <row spans="1:13" r="1">
-      <c r="A1" t="s">
+    <row spans="1:14" r="1">
+      <c t="s" r="A1">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c t="s" r="L1">
         <v>10</v>
       </c>
+      <c t="n" r="N1">
+        <v>0</v>
+      </c>
     </row>
-    <row spans="1:13" r="2">
-      <c r="A2" t="s">
+    <row spans="1:14" r="2">
+      <c t="s" r="A2">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>8</v>
       </c>
-      <c r="G2" t="n">
+      <c t="n" r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c t="s" r="H2">
         <v>2</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="J2">
         <v>8</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c t="s" r="L2">
         <v>8</v>
       </c>
-      <c r="M2" t="n">
+      <c t="n" r="M2">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:13" r="3">
-      <c r="F3" t="s">
+    <row spans="1:14" r="3">
+      <c t="s" r="F3">
         <v>7</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="H3">
         <v>8</v>
       </c>
-      <c r="I3" t="n">
+      <c t="n" r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c t="s" r="J3">
         <v>7</v>
       </c>
-      <c r="K3" t="n">
+      <c t="n" r="K3">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c t="s" r="L3">
         <v>7</v>
       </c>
-      <c r="M3" t="n">
+      <c t="n" r="M3">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:13" r="4">
-      <c r="H4" t="s">
+    <row spans="1:14" r="4">
+      <c t="s" r="H4">
         <v>7</v>
       </c>
-      <c r="I4" t="n">
+      <c t="n" r="I4">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistical significance passing tests
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="ExistingData" r:id="rId1" sheetId="1"/>
     <sheet name="DisplayValues" r:id="rId2" sheetId="2"/>
-    <sheet name="Lookups" r:id="rId3" sheetId="3"/>
+    <sheet name="SignificanceValues" r:id="rId3" sheetId="3"/>
+    <sheet name="Lookups" r:id="rId4" sheetId="4"/>
   </sheets>
   <definedNames>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Corps</t>
   </si>
@@ -45,10 +46,16 @@
     <t>Grade</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
   <si>
     <t>female</t>
@@ -426,14 +433,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col width="9.1" min="3" customWidth="true" max="3"/>
+    <col width="9.1" min="2" customWidth="true" max="2"/>
+    <col width="9.1" min="1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c t="n" r="B1">
         <v>2.3</v>
@@ -469,6 +476,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col width="9.1" min="3" customWidth="true" max="3"/>
+    <col width="9.1" min="2" customWidth="true" max="2"/>
+    <col width="9.1" min="1" customWidth="true" max="1"/>
+  </cols>
+  <sheetData>
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
+        <v>13</v>
+      </c>
+      <c t="n" r="B1">
+        <v>2.3</v>
+      </c>
+      <c t="n" r="C1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
+        <v>0</v>
+      </c>
+      <c t="s" r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
@@ -481,20 +537,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="12" width="9.10" min="12"/>
-    <col max="13" width="9.10" min="13"/>
-    <col max="14" width="9.10" min="14"/>
-    <col max="8" width="9.10" min="8"/>
-    <col max="9" width="9.10" min="9"/>
-    <col max="10" width="9.10" min="10"/>
-    <col max="11" width="9.10" min="11"/>
-    <col max="4" width="9.10" min="4"/>
-    <col max="5" width="9.10" min="5"/>
-    <col max="6" width="9.10" min="6"/>
-    <col max="7" width="9.10" min="7"/>
-    <col max="1" width="9.10" min="1"/>
-    <col max="2" width="9.10" min="2"/>
-    <col max="3" width="9.10" min="3"/>
+    <col width="9.10" min="11" max="11"/>
+    <col width="9.10" min="10" max="10"/>
+    <col width="9.10" min="9" max="9"/>
+    <col width="9.10" min="8" max="8"/>
+    <col width="9.10" min="14" max="14"/>
+    <col width="9.10" min="13" max="13"/>
+    <col width="9.10" min="12" max="12"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="7" max="7"/>
+    <col width="9.10" min="6" max="6"/>
+    <col width="9.10" min="5" max="5"/>
+    <col width="9.10" min="4" max="4"/>
   </cols>
   <sheetData>
     <row spans="1:14" r="1">
@@ -502,13 +558,13 @@
         <v>4</v>
       </c>
       <c t="s" r="B1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="C1">
         <v>4</v>
       </c>
       <c t="s" r="D1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="E1">
         <v>0</v>
@@ -520,10 +576,10 @@
         <v>3</v>
       </c>
       <c t="s" r="J1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c t="s" r="L1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c t="n" r="N1">
         <v>0</v>
@@ -531,22 +587,22 @@
     </row>
     <row spans="1:14" r="2">
       <c t="s" r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="B2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="D2">
         <v>0</v>
       </c>
       <c t="s" r="E2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c t="s" r="F2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c t="n" r="G2">
         <v>1</v>
@@ -558,13 +614,13 @@
         <v>0</v>
       </c>
       <c t="s" r="J2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c t="n" r="K2">
         <v>1</v>
       </c>
       <c t="s" r="L2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c t="n" r="M2">
         <v>1</v>
@@ -572,25 +628,25 @@
     </row>
     <row spans="1:14" r="3">
       <c t="s" r="F3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c t="n" r="G3">
         <v>2</v>
       </c>
       <c t="s" r="H3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c t="n" r="I3">
         <v>1</v>
       </c>
       <c t="s" r="J3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c t="n" r="K3">
         <v>2</v>
       </c>
       <c t="s" r="L3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c t="n" r="M3">
         <v>2</v>
@@ -598,7 +654,7 @@
     </row>
     <row spans="1:14" r="4">
       <c t="s" r="H4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c t="n" r="I4">
         <v>2</v>

</xml_diff>

<commit_message>
Added named ranges for significance values
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -16,6 +16,9 @@
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
     <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$3</definedName>
     <definedName name="disp_value_values">'DisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="sig_value_col_head">'SignificanceValues'!$B$1:$C$1</definedName>
+    <definedName name="sig_value_row_head">'SignificanceValues'!$A$2:$A$3</definedName>
+    <definedName name="sig_value_values">'SignificanceValues'!$B$2:$C$3</definedName>
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
@@ -412,7 +415,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -428,14 +431,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" min="3" customWidth="true" max="3"/>
-    <col width="9.1" min="2" customWidth="true" max="2"/>
-    <col width="9.1" min="1" customWidth="true" max="1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -483,14 +486,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" min="3" customWidth="true" max="3"/>
-    <col width="9.1" min="2" customWidth="true" max="2"/>
-    <col width="9.1" min="1" customWidth="true" max="1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -532,25 +535,25 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="11" max="11"/>
-    <col width="9.10" min="10" max="10"/>
-    <col width="9.10" min="9" max="9"/>
-    <col width="9.10" min="8" max="8"/>
-    <col width="9.10" min="14" max="14"/>
-    <col width="9.10" min="13" max="13"/>
-    <col width="9.10" min="12" max="12"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="7" max="7"/>
-    <col width="9.10" min="6" max="6"/>
-    <col width="9.10" min="5" max="5"/>
-    <col width="9.10" min="4" max="4"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
   </cols>
   <sheetData>
     <row spans="1:14" r="1">

</xml_diff>

<commit_message>
Output third column that shows associated dimension
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -24,15 +24,18 @@
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
     <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$M$1</definedName>
-    <definedName name="zero_string">'Lookups'!$N$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$P$1</definedName>
+    <definedName name="zero_string">'Lookups'!$Q$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+  <si>
+    <t>Atlanta</t>
+  </si>
   <si>
     <t>Corps</t>
   </si>
@@ -46,6 +49,9 @@
     <t>GenderB</t>
   </si>
   <si>
+    <t>GenderC</t>
+  </si>
+  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -59,6 +65,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>SoDak</t>
   </si>
   <si>
     <t>female</t>
@@ -410,7 +419,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
@@ -426,7 +435,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -436,14 +445,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="B1">
         <v>2.3</v>
@@ -481,7 +490,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -491,14 +500,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="B1">
         <v>2.3</v>
@@ -512,7 +521,7 @@
         <v>0</v>
       </c>
       <c t="s" r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row spans="1:3" r="3">
@@ -520,7 +529,7 @@
         <v>1</v>
       </c>
       <c t="s" r="C3">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -530,9 +539,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,127 +549,160 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="8" min="8" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="14" min="14" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
+    <col min="17" width="9.10" max="17"/>
+    <col min="16" width="9.10" max="16"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="3" width="9.10" max="3"/>
+    <col min="2" width="9.10" max="2"/>
+    <col min="5" width="9.10" max="5"/>
+    <col min="4" width="9.10" max="4"/>
+    <col min="7" width="9.10" max="7"/>
+    <col min="6" width="9.10" max="6"/>
+    <col min="9" width="9.10" max="9"/>
+    <col min="8" width="9.10" max="8"/>
+    <col min="11" width="9.10" max="11"/>
+    <col min="10" width="9.10" max="10"/>
+    <col min="13" width="9.10" max="13"/>
+    <col min="12" width="9.10" max="12"/>
+    <col min="15" width="9.10" max="15"/>
+    <col min="14" width="9.10" max="14"/>
   </cols>
   <sheetData>
-    <row spans="1:14" r="1">
+    <row spans="1:17" r="1">
       <c t="s" r="A1">
+        <v>6</v>
+      </c>
+      <c t="s" r="B1">
+        <v>17</v>
+      </c>
+      <c t="s" r="C1">
+        <v>6</v>
+      </c>
+      <c t="s" r="D1">
+        <v>9</v>
+      </c>
+      <c t="s" r="E1">
+        <v>1</v>
+      </c>
+      <c t="s" r="F1">
+        <v>2</v>
+      </c>
+      <c t="s" r="H1">
         <v>4</v>
       </c>
-      <c t="s" r="B1">
+      <c t="s" r="J1">
+        <v>5</v>
+      </c>
+      <c t="s" r="M1">
         <v>14</v>
       </c>
-      <c t="s" r="C1">
-        <v>4</v>
-      </c>
-      <c t="s" r="D1">
-        <v>7</v>
-      </c>
-      <c t="s" r="E1">
+      <c t="s" r="O1">
+        <v>15</v>
+      </c>
+      <c t="n" r="Q1">
         <v>0</v>
       </c>
-      <c t="s" r="F1">
-        <v>1</v>
-      </c>
-      <c t="s" r="H1">
+    </row>
+    <row spans="1:17" r="2">
+      <c t="s" r="A2">
+        <v>9</v>
+      </c>
+      <c t="s" r="B2">
+        <v>17</v>
+      </c>
+      <c t="s" r="C2">
+        <v>9</v>
+      </c>
+      <c t="s" r="D2">
+        <v>1</v>
+      </c>
+      <c t="s" r="E2">
+        <v>8</v>
+      </c>
+      <c t="s" r="F2">
+        <v>13</v>
+      </c>
+      <c t="n" r="G2">
+        <v>1</v>
+      </c>
+      <c t="s" r="H2">
         <v>3</v>
-      </c>
-      <c t="s" r="J1">
-        <v>11</v>
-      </c>
-      <c t="s" r="L1">
-        <v>12</v>
-      </c>
-      <c t="n" r="N1">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:14" r="2">
-      <c t="s" r="A2">
-        <v>7</v>
-      </c>
-      <c t="s" r="B2">
-        <v>14</v>
-      </c>
-      <c t="s" r="C2">
-        <v>7</v>
-      </c>
-      <c t="s" r="D2">
-        <v>0</v>
-      </c>
-      <c t="s" r="E2">
-        <v>6</v>
-      </c>
-      <c t="s" r="F2">
-        <v>10</v>
-      </c>
-      <c t="n" r="G2">
-        <v>1</v>
-      </c>
-      <c t="s" r="H2">
-        <v>2</v>
       </c>
       <c t="n" r="I2">
         <v>0</v>
       </c>
       <c t="s" r="J2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c t="n" r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="L2">
-        <v>10</v>
-      </c>
-      <c t="n" r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:14" r="3">
+        <v>0</v>
+      </c>
+      <c t="s" r="M2">
+        <v>13</v>
+      </c>
+      <c t="n" r="N2">
+        <v>1</v>
+      </c>
+      <c t="s" r="O2">
+        <v>13</v>
+      </c>
+      <c t="n" r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:17" r="3">
       <c t="s" r="F3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c t="n" r="G3">
         <v>2</v>
       </c>
       <c t="s" r="H3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c t="n" r="I3">
         <v>1</v>
       </c>
       <c t="s" r="J3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c t="n" r="K3">
+        <v>1</v>
+      </c>
+      <c t="s" r="L3">
+        <v>0</v>
+      </c>
+      <c t="s" r="M3">
+        <v>12</v>
+      </c>
+      <c t="n" r="N3">
         <v>2</v>
       </c>
-      <c t="s" r="L3">
-        <v>9</v>
-      </c>
-      <c t="n" r="M3">
+      <c t="s" r="O3">
+        <v>12</v>
+      </c>
+      <c t="n" r="P3">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:14" r="4">
+    <row spans="1:17" r="4">
       <c t="s" r="H4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c t="n" r="I4">
         <v>2</v>
+      </c>
+      <c t="s" r="J4">
+        <v>12</v>
+      </c>
+      <c t="n" r="K4">
+        <v>2</v>
+      </c>
+      <c t="s" r="L4">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Only add blank rows for dynamic dimensions if parent dimension is included
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -424,7 +424,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,14 +440,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -495,14 +495,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -544,28 +544,28 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="17" width="9.10" max="17"/>
-    <col min="16" width="9.10" max="16"/>
-    <col min="1" width="9.10" max="1"/>
-    <col min="3" width="9.10" max="3"/>
-    <col min="2" width="9.10" max="2"/>
-    <col min="5" width="9.10" max="5"/>
-    <col min="4" width="9.10" max="4"/>
-    <col min="7" width="9.10" max="7"/>
-    <col min="6" width="9.10" max="6"/>
-    <col min="9" width="9.10" max="9"/>
-    <col min="8" width="9.10" max="8"/>
-    <col min="11" width="9.10" max="11"/>
-    <col min="10" width="9.10" max="10"/>
-    <col min="13" width="9.10" max="13"/>
-    <col min="12" width="9.10" max="12"/>
-    <col min="15" width="9.10" max="15"/>
-    <col min="14" width="9.10" max="14"/>
+    <col max="16" width="9.10" min="16"/>
+    <col max="17" width="9.10" min="17"/>
+    <col max="1" width="9.10" min="1"/>
+    <col max="2" width="9.10" min="2"/>
+    <col max="3" width="9.10" min="3"/>
+    <col max="4" width="9.10" min="4"/>
+    <col max="5" width="9.10" min="5"/>
+    <col max="6" width="9.10" min="6"/>
+    <col max="7" width="9.10" min="7"/>
+    <col max="8" width="9.10" min="8"/>
+    <col max="9" width="9.10" min="9"/>
+    <col max="10" width="9.10" min="10"/>
+    <col max="11" width="9.10" min="11"/>
+    <col max="12" width="9.10" min="12"/>
+    <col max="13" width="9.10" min="13"/>
+    <col max="14" width="9.10" min="14"/>
+    <col max="15" width="9.10" min="15"/>
   </cols>
   <sheetData>
     <row spans="1:17" r="1">

</xml_diff>

<commit_message>
When creating menu for composite dimension, it's just a concatenation of component dimensions
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -24,15 +24,15 @@
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
     <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$P$1</definedName>
-    <definedName name="zero_string">'Lookups'!$Q$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$R$1</definedName>
+    <definedName name="zero_string">'Lookups'!$S$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Atlanta</t>
   </si>
@@ -52,6 +52,9 @@
     <t>GenderC</t>
   </si>
   <si>
+    <t>Gender_LIB</t>
+  </si>
+  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>lib</t>
   </si>
   <si>
     <t>male</t>
@@ -424,7 +430,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,46 +446,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col width="9.1" max="3" min="3" customWidth="true"/>
+    <col width="9.1" max="2" min="2" customWidth="true"/>
+    <col width="9.1" max="1" min="1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
-        <v>16</v>
-      </c>
-      <c t="n" r="B1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="n" r="B3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -495,41 +501,41 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col width="9.1" max="3" min="3" customWidth="true"/>
+    <col width="9.1" max="2" min="2" customWidth="true"/>
+    <col width="9.1" max="1" min="1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
-        <v>16</v>
-      </c>
-      <c t="n" r="B1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="B2">
-        <v>7</v>
-      </c>
-    </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="s" r="C3">
-        <v>10</v>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -541,168 +547,191 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="16" width="9.10" min="16"/>
-    <col max="17" width="9.10" min="17"/>
-    <col max="1" width="9.10" min="1"/>
-    <col max="2" width="9.10" min="2"/>
-    <col max="3" width="9.10" min="3"/>
-    <col max="4" width="9.10" min="4"/>
-    <col max="5" width="9.10" min="5"/>
-    <col max="6" width="9.10" min="6"/>
-    <col max="7" width="9.10" min="7"/>
-    <col max="8" width="9.10" min="8"/>
-    <col max="9" width="9.10" min="9"/>
-    <col max="10" width="9.10" min="10"/>
-    <col max="11" width="9.10" min="11"/>
-    <col max="12" width="9.10" min="12"/>
-    <col max="13" width="9.10" min="13"/>
-    <col max="14" width="9.10" min="14"/>
-    <col max="15" width="9.10" min="15"/>
+    <col width="9.10" max="19" min="19"/>
+    <col width="9.10" max="18" min="18"/>
+    <col width="9.10" max="17" min="17"/>
+    <col width="9.10" max="16" min="16"/>
+    <col width="9.10" max="7" min="7"/>
+    <col width="9.10" max="6" min="6"/>
+    <col width="9.10" max="5" min="5"/>
+    <col width="9.10" max="4" min="4"/>
+    <col width="9.10" max="3" min="3"/>
+    <col width="9.10" max="2" min="2"/>
+    <col width="9.10" max="1" min="1"/>
+    <col width="9.10" max="15" min="15"/>
+    <col width="9.10" max="14" min="14"/>
+    <col width="9.10" max="13" min="13"/>
+    <col width="9.10" max="12" min="12"/>
+    <col width="9.10" max="11" min="11"/>
+    <col width="9.10" max="10" min="10"/>
+    <col width="9.10" max="9" min="9"/>
+    <col width="9.10" max="8" min="8"/>
   </cols>
   <sheetData>
-    <row spans="1:17" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="B1">
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C1">
-        <v>6</v>
-      </c>
-      <c t="s" r="D1">
+      <c r="S1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="E1">
-        <v>1</v>
-      </c>
-      <c t="s" r="F1">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="H1">
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="n">
         <v>4</v>
-      </c>
-      <c t="s" r="J1">
-        <v>5</v>
-      </c>
-      <c t="s" r="M1">
-        <v>14</v>
-      </c>
-      <c t="s" r="O1">
-        <v>15</v>
-      </c>
-      <c t="n" r="Q1">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:17" r="2">
-      <c t="s" r="A2">
-        <v>9</v>
-      </c>
-      <c t="s" r="B2">
-        <v>17</v>
-      </c>
-      <c t="s" r="C2">
-        <v>9</v>
-      </c>
-      <c t="s" r="D2">
-        <v>1</v>
-      </c>
-      <c t="s" r="E2">
-        <v>8</v>
-      </c>
-      <c t="s" r="F2">
-        <v>13</v>
-      </c>
-      <c t="n" r="G2">
-        <v>1</v>
-      </c>
-      <c t="s" r="H2">
-        <v>3</v>
-      </c>
-      <c t="n" r="I2">
-        <v>0</v>
-      </c>
-      <c t="s" r="J2">
-        <v>12</v>
-      </c>
-      <c t="n" r="K2">
-        <v>2</v>
-      </c>
-      <c t="s" r="L2">
-        <v>0</v>
-      </c>
-      <c t="s" r="M2">
-        <v>13</v>
-      </c>
-      <c t="n" r="N2">
-        <v>1</v>
-      </c>
-      <c t="s" r="O2">
-        <v>13</v>
-      </c>
-      <c t="n" r="P2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:17" r="3">
-      <c t="s" r="F3">
-        <v>12</v>
-      </c>
-      <c t="n" r="G3">
-        <v>2</v>
-      </c>
-      <c t="s" r="H3">
-        <v>13</v>
-      </c>
-      <c t="n" r="I3">
-        <v>1</v>
-      </c>
-      <c t="s" r="J3">
-        <v>13</v>
-      </c>
-      <c t="n" r="K3">
-        <v>1</v>
-      </c>
-      <c t="s" r="L3">
-        <v>0</v>
-      </c>
-      <c t="s" r="M3">
-        <v>12</v>
-      </c>
-      <c t="n" r="N3">
-        <v>2</v>
-      </c>
-      <c t="s" r="O3">
-        <v>12</v>
-      </c>
-      <c t="n" r="P3">
-        <v>2</v>
-      </c>
-    </row>
-    <row spans="1:17" r="4">
-      <c t="s" r="H4">
-        <v>12</v>
-      </c>
-      <c t="n" r="I4">
-        <v>2</v>
-      </c>
-      <c t="s" r="J4">
-        <v>12</v>
-      </c>
-      <c t="n" r="K4">
-        <v>2</v>
-      </c>
-      <c t="s" r="L4">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making change to how demographics are computed
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -451,41 +451,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="3" min="3" customWidth="true"/>
-    <col width="9.1" max="2" min="2" customWidth="true"/>
-    <col width="9.1" max="1" min="1" customWidth="true"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>18</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -506,35 +506,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="3" min="3" customWidth="true"/>
-    <col width="9.1" max="2" min="2" customWidth="true"/>
-    <col width="9.1" max="1" min="1" customWidth="true"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>18</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
         <v>11</v>
       </c>
     </row>
@@ -555,182 +555,182 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="19" min="19"/>
-    <col width="9.10" max="18" min="18"/>
-    <col width="9.10" max="17" min="17"/>
-    <col width="9.10" max="16" min="16"/>
-    <col width="9.10" max="7" min="7"/>
-    <col width="9.10" max="6" min="6"/>
-    <col width="9.10" max="5" min="5"/>
-    <col width="9.10" max="4" min="4"/>
-    <col width="9.10" max="3" min="3"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="1" min="1"/>
-    <col width="9.10" max="15" min="15"/>
-    <col width="9.10" max="14" min="14"/>
-    <col width="9.10" max="13" min="13"/>
-    <col width="9.10" max="12" min="12"/>
-    <col width="9.10" max="11" min="11"/>
-    <col width="9.10" max="10" min="10"/>
-    <col width="9.10" max="9" min="9"/>
-    <col width="9.10" max="8" min="8"/>
+    <col max="1" width="9.10" min="1"/>
+    <col max="2" width="9.10" min="2"/>
+    <col max="3" width="9.10" min="3"/>
+    <col max="4" width="9.10" min="4"/>
+    <col max="5" width="9.10" min="5"/>
+    <col max="6" width="9.10" min="6"/>
+    <col max="7" width="9.10" min="7"/>
+    <col max="8" width="9.10" min="8"/>
+    <col max="9" width="9.10" min="9"/>
+    <col max="10" width="9.10" min="10"/>
+    <col max="11" width="9.10" min="11"/>
+    <col max="12" width="9.10" min="12"/>
+    <col max="13" width="9.10" min="13"/>
+    <col max="14" width="9.10" min="14"/>
+    <col max="15" width="9.10" min="15"/>
+    <col max="16" width="9.10" min="16"/>
+    <col max="17" width="9.10" min="17"/>
+    <col max="18" width="9.10" min="18"/>
+    <col max="19" width="9.10" min="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" t="s">
+    <row spans="1:19" r="1">
+      <c t="s" r="A1">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c t="s" r="E1">
+        <v>1</v>
+      </c>
+      <c t="s" r="F1">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="H1">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="J1">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c t="s" r="M1">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c t="s" r="O1">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c t="s" r="Q1">
         <v>17</v>
       </c>
-      <c r="S1" t="n">
+      <c t="n" r="S1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" t="s">
+    <row spans="1:19" r="2">
+      <c t="s" r="A2">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c t="s" r="D2">
+        <v>1</v>
+      </c>
+      <c t="s" r="E2">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>15</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c t="n" r="G2">
+        <v>1</v>
+      </c>
+      <c t="s" r="H2">
         <v>3</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="J2">
         <v>13</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="K2">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
+      <c t="s" r="L2">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c t="s" r="M2">
         <v>15</v>
       </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c t="n" r="N2">
+        <v>1</v>
+      </c>
+      <c t="s" r="O2">
         <v>15</v>
       </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
+      <c t="n" r="P2">
+        <v>1</v>
+      </c>
+      <c t="s" r="Q2">
         <v>15</v>
       </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="F3" t="s">
+      <c t="n" r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:19" r="3">
+      <c t="s" r="F3">
         <v>13</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="G3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="H3">
         <v>15</v>
       </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
+      <c t="n" r="I3">
+        <v>1</v>
+      </c>
+      <c t="s" r="J3">
         <v>15</v>
       </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c t="n" r="K3">
+        <v>1</v>
+      </c>
+      <c t="s" r="L3">
         <v>0</v>
       </c>
-      <c r="M3" t="s">
+      <c t="s" r="M3">
         <v>13</v>
       </c>
-      <c r="N3" t="n">
+      <c t="n" r="N3">
         <v>2</v>
       </c>
-      <c r="O3" t="s">
+      <c t="s" r="O3">
         <v>13</v>
       </c>
-      <c r="P3" t="n">
+      <c t="n" r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" t="s">
+      <c t="s" r="Q3">
         <v>13</v>
       </c>
-      <c r="R3" t="n">
+      <c t="n" r="R3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="H4" t="s">
+    <row spans="1:19" r="4">
+      <c t="s" r="H4">
         <v>13</v>
       </c>
-      <c r="I4" t="n">
+      <c t="n" r="I4">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c t="s" r="J4">
         <v>13</v>
       </c>
-      <c r="K4" t="n">
+      <c t="n" r="K4">
         <v>2</v>
       </c>
-      <c r="L4" t="s">
+      <c t="s" r="L4">
         <v>12</v>
       </c>
-      <c r="M4" t="s">
+      <c t="s" r="M4">
         <v>14</v>
       </c>
-      <c r="N4" t="n">
+      <c t="n" r="N4">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
If order of values in dimensions is specified, use those values
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -24,19 +24,25 @@
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
     <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$R$1</definedName>
-    <definedName name="zero_string">'Lookups'!$S$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$F$1:$T$1</definedName>
+    <definedName name="zero_string">'Lookups'!$U$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+  <si>
+    <t>A</t>
+  </si>
   <si>
     <t>Atlanta</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>Corps</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t>SoDak</t>
+  </si>
+  <si>
+    <t>ValueOrderDimension</t>
   </si>
   <si>
     <t>female</t>
@@ -430,7 +439,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,19 +455,19 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col width="9.1" min="3" customWidth="true" max="3"/>
+    <col width="9.1" min="2" customWidth="true" max="2"/>
+    <col width="9.1" min="1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c t="n" r="B1">
         <v>2.3</v>
@@ -501,19 +510,19 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col width="9.1" min="3" customWidth="true" max="3"/>
+    <col width="9.1" min="2" customWidth="true" max="2"/>
+    <col width="9.1" min="1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c t="n" r="B1">
         <v>2.3</v>
@@ -527,7 +536,7 @@
         <v>0</v>
       </c>
       <c t="s" r="B2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row spans="1:3" r="3">
@@ -535,7 +544,7 @@
         <v>1</v>
       </c>
       <c t="s" r="C3">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -547,188 +556,205 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" width="9.10" min="1"/>
-    <col max="2" width="9.10" min="2"/>
-    <col max="3" width="9.10" min="3"/>
-    <col max="4" width="9.10" min="4"/>
-    <col max="5" width="9.10" min="5"/>
-    <col max="6" width="9.10" min="6"/>
-    <col max="7" width="9.10" min="7"/>
-    <col max="8" width="9.10" min="8"/>
-    <col max="9" width="9.10" min="9"/>
-    <col max="10" width="9.10" min="10"/>
-    <col max="11" width="9.10" min="11"/>
-    <col max="12" width="9.10" min="12"/>
-    <col max="13" width="9.10" min="13"/>
-    <col max="14" width="9.10" min="14"/>
-    <col max="15" width="9.10" min="15"/>
-    <col max="16" width="9.10" min="16"/>
-    <col max="17" width="9.10" min="17"/>
-    <col max="18" width="9.10" min="18"/>
-    <col max="19" width="9.10" min="19"/>
+    <col width="9.10" min="11" max="11"/>
+    <col width="9.10" min="10" max="10"/>
+    <col width="9.10" min="9" max="9"/>
+    <col width="9.10" min="8" max="8"/>
+    <col width="9.10" min="15" max="15"/>
+    <col width="9.10" min="14" max="14"/>
+    <col width="9.10" min="13" max="13"/>
+    <col width="9.10" min="12" max="12"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="7" max="7"/>
+    <col width="9.10" min="6" max="6"/>
+    <col width="9.10" min="5" max="5"/>
+    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="19" max="19"/>
+    <col width="9.10" min="18" max="18"/>
+    <col width="9.10" min="17" max="17"/>
+    <col width="9.10" min="16" max="16"/>
+    <col width="9.10" min="21" max="21"/>
+    <col width="9.10" min="20" max="20"/>
   </cols>
   <sheetData>
-    <row spans="1:19" r="1">
+    <row spans="1:21" r="1">
       <c t="s" r="A1">
+        <v>9</v>
+      </c>
+      <c t="s" r="B1">
+        <v>22</v>
+      </c>
+      <c t="s" r="C1">
+        <v>9</v>
+      </c>
+      <c t="s" r="D1">
+        <v>12</v>
+      </c>
+      <c t="s" r="E1">
+        <v>3</v>
+      </c>
+      <c t="s" r="F1">
+        <v>4</v>
+      </c>
+      <c t="s" r="H1">
+        <v>6</v>
+      </c>
+      <c t="s" r="J1">
         <v>7</v>
       </c>
-      <c t="s" r="B1">
+      <c t="s" r="M1">
+        <v>8</v>
+      </c>
+      <c t="s" r="O1">
+        <v>15</v>
+      </c>
+      <c t="s" r="Q1">
         <v>19</v>
       </c>
-      <c t="s" r="C1">
-        <v>7</v>
-      </c>
-      <c t="s" r="D1">
-        <v>10</v>
-      </c>
-      <c t="s" r="E1">
-        <v>1</v>
-      </c>
-      <c t="s" r="F1">
-        <v>2</v>
-      </c>
-      <c t="s" r="H1">
-        <v>4</v>
-      </c>
-      <c t="s" r="J1">
+      <c t="s" r="S1">
+        <v>20</v>
+      </c>
+      <c t="n" r="U1">
+        <v>0</v>
+      </c>
+    </row>
+    <row spans="1:21" r="2">
+      <c t="s" r="A2">
+        <v>12</v>
+      </c>
+      <c t="s" r="B2">
+        <v>22</v>
+      </c>
+      <c t="s" r="C2">
+        <v>12</v>
+      </c>
+      <c t="s" r="D2">
+        <v>3</v>
+      </c>
+      <c t="s" r="E2">
+        <v>11</v>
+      </c>
+      <c t="s" r="F2">
+        <v>18</v>
+      </c>
+      <c t="n" r="G2">
+        <v>1</v>
+      </c>
+      <c t="s" r="H2">
         <v>5</v>
-      </c>
-      <c t="s" r="M1">
-        <v>6</v>
-      </c>
-      <c t="s" r="O1">
-        <v>16</v>
-      </c>
-      <c t="s" r="Q1">
-        <v>17</v>
-      </c>
-      <c t="n" r="S1">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:19" r="2">
-      <c t="s" r="A2">
-        <v>10</v>
-      </c>
-      <c t="s" r="B2">
-        <v>19</v>
-      </c>
-      <c t="s" r="C2">
-        <v>10</v>
-      </c>
-      <c t="s" r="D2">
-        <v>1</v>
-      </c>
-      <c t="s" r="E2">
-        <v>9</v>
-      </c>
-      <c t="s" r="F2">
-        <v>15</v>
-      </c>
-      <c t="n" r="G2">
-        <v>1</v>
-      </c>
-      <c t="s" r="H2">
-        <v>3</v>
       </c>
       <c t="n" r="I2">
         <v>0</v>
       </c>
       <c t="s" r="J2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="K2">
         <v>2</v>
       </c>
       <c t="s" r="L2">
+        <v>1</v>
+      </c>
+      <c t="s" r="M2">
+        <v>18</v>
+      </c>
+      <c t="n" r="N2">
+        <v>1</v>
+      </c>
+      <c t="s" r="O2">
+        <v>2</v>
+      </c>
+      <c t="n" r="P2">
+        <v>2</v>
+      </c>
+      <c t="s" r="Q2">
+        <v>18</v>
+      </c>
+      <c t="n" r="R2">
+        <v>1</v>
+      </c>
+      <c t="s" r="S2">
+        <v>18</v>
+      </c>
+      <c t="n" r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:21" r="3">
+      <c t="s" r="F3">
+        <v>16</v>
+      </c>
+      <c t="n" r="G3">
+        <v>2</v>
+      </c>
+      <c t="s" r="H3">
+        <v>18</v>
+      </c>
+      <c t="n" r="I3">
+        <v>1</v>
+      </c>
+      <c t="s" r="J3">
+        <v>18</v>
+      </c>
+      <c t="n" r="K3">
+        <v>1</v>
+      </c>
+      <c t="s" r="L3">
+        <v>1</v>
+      </c>
+      <c t="s" r="M3">
+        <v>16</v>
+      </c>
+      <c t="n" r="N3">
+        <v>2</v>
+      </c>
+      <c t="s" r="O3">
         <v>0</v>
       </c>
-      <c t="s" r="M2">
-        <v>15</v>
-      </c>
-      <c t="n" r="N2">
-        <v>1</v>
-      </c>
-      <c t="s" r="O2">
-        <v>15</v>
-      </c>
-      <c t="n" r="P2">
-        <v>1</v>
-      </c>
-      <c t="s" r="Q2">
-        <v>15</v>
-      </c>
-      <c t="n" r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:19" r="3">
-      <c t="s" r="F3">
-        <v>13</v>
-      </c>
-      <c t="n" r="G3">
-        <v>2</v>
-      </c>
-      <c t="s" r="H3">
-        <v>15</v>
-      </c>
-      <c t="n" r="I3">
-        <v>1</v>
-      </c>
-      <c t="s" r="J3">
-        <v>15</v>
-      </c>
-      <c t="n" r="K3">
-        <v>1</v>
-      </c>
-      <c t="s" r="L3">
-        <v>0</v>
-      </c>
-      <c t="s" r="M3">
-        <v>13</v>
-      </c>
-      <c t="n" r="N3">
-        <v>2</v>
-      </c>
-      <c t="s" r="O3">
-        <v>13</v>
-      </c>
       <c t="n" r="P3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c t="s" r="Q3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="R3">
         <v>2</v>
       </c>
-    </row>
-    <row spans="1:19" r="4">
+      <c t="s" r="S3">
+        <v>16</v>
+      </c>
+      <c t="n" r="T3">
+        <v>2</v>
+      </c>
+    </row>
+    <row spans="1:21" r="4">
       <c t="s" r="H4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="I4">
         <v>2</v>
       </c>
       <c t="s" r="J4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c t="n" r="K4">
         <v>2</v>
       </c>
       <c t="s" r="L4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="M4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c t="n" r="N4">
         <v>4</v>

</xml_diff>

<commit_message>
Copy of create from config that does historical stuff (include new input of results and demographics)
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -10,7 +10,9 @@
     <sheet name="ExistingData" r:id="rId1" sheetId="1"/>
     <sheet name="DisplayValues" r:id="rId2" sheetId="2"/>
     <sheet name="SignificanceValues" r:id="rId3" sheetId="3"/>
-    <sheet name="Lookups" r:id="rId4" sheetId="4"/>
+    <sheet name="HistDisplayValues" r:id="rId4" sheetId="4"/>
+    <sheet name="HistSignificanceValues" r:id="rId5" sheetId="5"/>
+    <sheet name="Lookups" r:id="rId6" sheetId="6"/>
   </sheets>
   <definedNames>
     <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
@@ -19,6 +21,12 @@
     <definedName name="sig_value_col_head">'SignificanceValues'!$B$1:$C$1</definedName>
     <definedName name="sig_value_row_head">'SignificanceValues'!$A$2:$A$3</definedName>
     <definedName name="sig_value_values">'SignificanceValues'!$B$2:$C$3</definedName>
+    <definedName name="hist_disp_value_col_head">'HistDisplayValues'!$B$1:$C$1</definedName>
+    <definedName name="hist_disp_value_row_head">'HistDisplayValues'!$A$2:$A$3</definedName>
+    <definedName name="hist_disp_value_values">'HistDisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="hist_sig_value_col_head">'HistSignificanceValues'!$B$1:$C$1</definedName>
+    <definedName name="hist_sig_value_row_head">'HistSignificanceValues'!$A$2:$A$3</definedName>
+    <definedName name="hist_sig_value_values">'HistSignificanceValues'!$B$2:$C$3</definedName>
     <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
     <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
@@ -432,14 +440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -448,53 +456,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" min="3" customWidth="true" max="3"/>
-    <col width="9.1" min="2" customWidth="true" max="2"/>
-    <col width="9.1" min="1" customWidth="true" max="1"/>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="n" r="B3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -503,47 +511,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" min="3" customWidth="true" max="3"/>
-    <col width="9.1" min="2" customWidth="true" max="2"/>
-    <col width="9.1" min="1" customWidth="true" max="1"/>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>2.3</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="s" r="C3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -552,211 +560,315 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col width="9.10" min="14" max="14"/>
+    <col width="9.10" min="15" max="15"/>
+    <col width="9.10" min="12" max="12"/>
+    <col width="9.10" min="13" max="13"/>
+    <col width="9.10" min="10" max="10"/>
     <col width="9.10" min="11" max="11"/>
-    <col width="9.10" min="10" max="10"/>
+    <col width="9.10" min="8" max="8"/>
     <col width="9.10" min="9" max="9"/>
-    <col width="9.10" min="8" max="8"/>
-    <col width="9.10" min="15" max="15"/>
-    <col width="9.10" min="14" max="14"/>
-    <col width="9.10" min="13" max="13"/>
-    <col width="9.10" min="12" max="12"/>
+    <col width="9.10" min="6" max="6"/>
+    <col width="9.10" min="7" max="7"/>
+    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="5" max="5"/>
+    <col width="9.10" min="2" max="2"/>
     <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="2" max="2"/>
     <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="7" max="7"/>
-    <col width="9.10" min="6" max="6"/>
-    <col width="9.10" min="5" max="5"/>
-    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="20" max="20"/>
+    <col width="9.10" min="21" max="21"/>
+    <col width="9.10" min="18" max="18"/>
     <col width="9.10" min="19" max="19"/>
-    <col width="9.10" min="18" max="18"/>
+    <col width="9.10" min="16" max="16"/>
     <col width="9.10" min="17" max="17"/>
-    <col width="9.10" min="16" max="16"/>
-    <col width="9.10" min="21" max="21"/>
-    <col width="9.10" min="20" max="20"/>
   </cols>
   <sheetData>
-    <row spans="1:21" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="M1">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="O1">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="Q1">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="S1">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="U1">
+      <c r="U1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:21" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="G2">
-        <v>1</v>
-      </c>
-      <c t="s" r="H2">
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="I2">
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="J2">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="K2">
+      <c r="K2" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="L2">
-        <v>1</v>
-      </c>
-      <c t="s" r="M2">
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="N2">
-        <v>1</v>
-      </c>
-      <c t="s" r="O2">
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>2</v>
       </c>
-      <c t="n" r="P2">
+      <c r="P2" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="Q2">
+      <c r="Q2" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="R2">
-        <v>1</v>
-      </c>
-      <c t="s" r="S2">
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="T2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:21" r="3">
-      <c t="s" r="F3">
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="G3">
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="H3">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="I3">
-        <v>1</v>
-      </c>
-      <c t="s" r="J3">
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="K3">
-        <v>1</v>
-      </c>
-      <c t="s" r="L3">
-        <v>1</v>
-      </c>
-      <c t="s" r="M3">
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="N3">
+      <c r="N3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="O3">
+      <c r="O3" t="s">
         <v>0</v>
       </c>
-      <c t="n" r="P3">
-        <v>1</v>
-      </c>
-      <c t="s" r="Q3">
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="R3">
+      <c r="R3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="S3">
+      <c r="S3" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="T3">
+      <c r="T3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:21" r="4">
-      <c t="s" r="H4">
+    <row r="4" spans="1:21">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="I4">
+      <c r="I4" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="J4">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="K4">
+      <c r="K4" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="L4">
+      <c r="L4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="M4">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c t="n" r="N4">
+      <c r="N4" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Menu item on cuts create seperate menu for each config
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -27,13 +27,14 @@
     <definedName name="hist_sig_value_col_head">'HistSignificanceValues'!$B$1:$C$1</definedName>
     <definedName name="hist_sig_value_row_head">'HistSignificanceValues'!$A$2:$A$3</definedName>
     <definedName name="hist_sig_value_values">'HistSignificanceValues'!$B$2:$C$3</definedName>
-    <definedName name="cuts">'Lookups'!$A$1:$A$2</definedName>
     <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
-    <definedName name="default_menu">'Lookups'!$E$2:$E$101</definedName>
-    <definedName name="default_mapping">'Lookups'!$E$2:$F$101</definedName>
-    <definedName name="default_menu_start">'Lookups'!$E$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$F$1:$T$1</definedName>
-    <definedName name="zero_string">'Lookups'!$U$1</definedName>
+    <definedName name="cuts">'Lookups'!$F$1:$F$2</definedName>
+    <definedName name="cuts_historical">'Lookups'!$F$3:$F$3</definedName>
+    <definedName name="default_menu">'Lookups'!$F$2:$F$101</definedName>
+    <definedName name="default_mapping">'Lookups'!$F$2:$G$101</definedName>
+    <definedName name="default_menu_start">'Lookups'!$F$2</definedName>
+    <definedName name="cuts_head">'Lookups'!$G$1:$U$1</definedName>
+    <definedName name="zero_string">'Lookups'!$V$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
@@ -440,14 +441,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -456,53 +457,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>21</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -511,47 +512,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>21</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
         <v>13</v>
       </c>
     </row>
@@ -560,53 +561,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>21</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -615,47 +616,47 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col width="9.1" max="1" customWidth="true" min="1"/>
+    <col width="9.1" max="2" customWidth="true" min="2"/>
+    <col width="9.1" max="3" customWidth="true" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>21</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>2.3</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row spans="1:3" r="2">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row spans="1:3" r="3">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
         <v>13</v>
       </c>
     </row>
@@ -664,211 +665,221 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="14" max="14"/>
-    <col width="9.10" min="15" max="15"/>
-    <col width="9.10" min="12" max="12"/>
-    <col width="9.10" min="13" max="13"/>
-    <col width="9.10" min="10" max="10"/>
-    <col width="9.10" min="11" max="11"/>
-    <col width="9.10" min="8" max="8"/>
-    <col width="9.10" min="9" max="9"/>
-    <col width="9.10" min="6" max="6"/>
-    <col width="9.10" min="7" max="7"/>
-    <col width="9.10" min="4" max="4"/>
-    <col width="9.10" min="5" max="5"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="20" max="20"/>
-    <col width="9.10" min="21" max="21"/>
-    <col width="9.10" min="18" max="18"/>
-    <col width="9.10" min="19" max="19"/>
-    <col width="9.10" min="16" max="16"/>
-    <col width="9.10" min="17" max="17"/>
+    <col width="9.10" max="20" min="20"/>
+    <col width="9.10" max="21" min="21"/>
+    <col width="9.10" max="22" min="22"/>
+    <col width="9.10" max="16" min="16"/>
+    <col width="9.10" max="17" min="17"/>
+    <col width="9.10" max="18" min="18"/>
+    <col width="9.10" max="19" min="19"/>
+    <col width="9.10" max="12" min="12"/>
+    <col width="9.10" max="13" min="13"/>
+    <col width="9.10" max="14" min="14"/>
+    <col width="9.10" max="15" min="15"/>
+    <col width="9.10" max="8" min="8"/>
+    <col width="9.10" max="9" min="9"/>
+    <col width="9.10" max="10" min="10"/>
+    <col width="9.10" max="11" min="11"/>
+    <col width="9.10" max="4" min="4"/>
+    <col width="9.10" max="5" min="5"/>
+    <col width="9.10" max="6" min="6"/>
+    <col width="9.10" max="7" min="7"/>
+    <col width="9.10" max="1" min="1"/>
+    <col width="9.10" max="2" min="2"/>
+    <col width="9.10" max="3" min="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" t="s">
+    <row spans="1:22" r="1">
+      <c t="s" r="A1">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
+        <v>9</v>
+      </c>
+      <c t="s" r="G1">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c t="s" r="I1">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c t="s" r="K1">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c t="s" r="N1">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c t="s" r="P1">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c t="s" r="R1">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c t="s" r="T1">
         <v>20</v>
       </c>
-      <c r="U1" t="n">
+      <c t="n" r="V1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
+    <row spans="1:22" r="2">
+      <c t="s" r="A2">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
+        <v>12</v>
+      </c>
+      <c t="s" r="G2">
         <v>18</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c t="n" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I2">
         <v>5</v>
       </c>
-      <c r="I2" t="n">
+      <c t="n" r="J2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c t="s" r="K2">
         <v>16</v>
       </c>
-      <c r="K2" t="n">
+      <c t="n" r="L2">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+      <c t="s" r="M2">
+        <v>1</v>
+      </c>
+      <c t="s" r="N2">
         <v>18</v>
       </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c t="n" r="O2">
+        <v>1</v>
+      </c>
+      <c t="s" r="P2">
         <v>2</v>
       </c>
-      <c r="P2" t="n">
+      <c t="n" r="Q2">
         <v>2</v>
       </c>
-      <c r="Q2" t="s">
+      <c t="s" r="R2">
         <v>18</v>
       </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
+      <c t="n" r="S2">
+        <v>1</v>
+      </c>
+      <c t="s" r="T2">
         <v>18</v>
       </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="F3" t="s">
+      <c t="n" r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:22" r="3">
+      <c t="s" r="F3">
+        <v>12</v>
+      </c>
+      <c t="s" r="G3">
         <v>16</v>
       </c>
-      <c r="G3" t="n">
+      <c t="n" r="H3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c t="s" r="I3">
         <v>18</v>
       </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
+      <c t="n" r="J3">
+        <v>1</v>
+      </c>
+      <c t="s" r="K3">
         <v>18</v>
       </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
+      <c t="n" r="L3">
+        <v>1</v>
+      </c>
+      <c t="s" r="M3">
+        <v>1</v>
+      </c>
+      <c t="s" r="N3">
         <v>16</v>
       </c>
-      <c r="N3" t="n">
+      <c t="n" r="O3">
         <v>2</v>
       </c>
-      <c r="O3" t="s">
+      <c t="s" r="P3">
         <v>0</v>
       </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
+      <c t="n" r="Q3">
+        <v>1</v>
+      </c>
+      <c t="s" r="R3">
         <v>16</v>
       </c>
-      <c r="R3" t="n">
+      <c t="n" r="S3">
         <v>2</v>
       </c>
-      <c r="S3" t="s">
+      <c t="s" r="T3">
         <v>16</v>
       </c>
-      <c r="T3" t="n">
+      <c t="n" r="U3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
-      <c r="H4" t="s">
+    <row spans="1:22" r="4">
+      <c t="s" r="I4">
         <v>16</v>
       </c>
-      <c r="I4" t="n">
+      <c t="n" r="J4">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c t="s" r="K4">
         <v>16</v>
       </c>
-      <c r="K4" t="n">
+      <c t="n" r="L4">
         <v>2</v>
       </c>
-      <c r="L4" t="s">
+      <c t="s" r="M4">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
+      <c t="s" r="N4">
         <v>17</v>
       </c>
-      <c r="N4" t="n">
+      <c t="n" r="O4">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix errors caused by pandas upgrade
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -33,15 +33,15 @@
     <definedName name="default_menu">'Lookups'!$F$2:$F$101</definedName>
     <definedName name="default_mapping">'Lookups'!$F$2:$G$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$F$2</definedName>
-    <definedName name="cuts_head">'Lookups'!$G$1:$U$1</definedName>
-    <definedName name="zero_string">'Lookups'!$V$1</definedName>
+    <definedName name="cuts_head">'Lookups'!$G$1:$W$1</definedName>
+    <definedName name="zero_string">'Lookups'!$X$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>static</t>
+  </si>
+  <si>
+    <t>survey_code</t>
   </si>
 </sst>
 </file>
@@ -441,14 +444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,21 +460,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -512,21 +515,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -561,21 +564,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -616,21 +619,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" max="1" customWidth="true" min="1"/>
-    <col width="9.1" max="2" customWidth="true" min="2"/>
-    <col width="9.1" max="3" customWidth="true" min="3"/>
+    <col customWidth="true" max="1" min="1" width="9.1"/>
+    <col customWidth="true" max="3" min="3" width="9.1"/>
+    <col customWidth="true" max="2" min="2" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
@@ -665,43 +668,45 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="20" min="20"/>
-    <col width="9.10" max="21" min="21"/>
-    <col width="9.10" max="22" min="22"/>
-    <col width="9.10" max="16" min="16"/>
-    <col width="9.10" max="17" min="17"/>
-    <col width="9.10" max="18" min="18"/>
-    <col width="9.10" max="19" min="19"/>
-    <col width="9.10" max="12" min="12"/>
-    <col width="9.10" max="13" min="13"/>
-    <col width="9.10" max="14" min="14"/>
-    <col width="9.10" max="15" min="15"/>
-    <col width="9.10" max="8" min="8"/>
-    <col width="9.10" max="9" min="9"/>
-    <col width="9.10" max="10" min="10"/>
-    <col width="9.10" max="11" min="11"/>
-    <col width="9.10" max="4" min="4"/>
-    <col width="9.10" max="5" min="5"/>
-    <col width="9.10" max="6" min="6"/>
-    <col width="9.10" max="7" min="7"/>
-    <col width="9.10" max="1" min="1"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="3" min="3"/>
+    <col max="24" min="24" width="9.10"/>
+    <col max="17" min="17" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
+    <col max="19" min="19" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="23" min="23" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:22" r="1">
+    <row spans="1:24" r="1">
       <c t="s" r="A1">
         <v>9</v>
       </c>
@@ -741,11 +746,14 @@
       <c t="s" r="T1">
         <v>20</v>
       </c>
-      <c t="n" r="V1">
+      <c t="s" r="V1">
+        <v>23</v>
+      </c>
+      <c t="n" r="X1">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:22" r="2">
+    <row spans="1:24" r="2">
       <c t="s" r="A2">
         <v>12</v>
       </c>
@@ -809,8 +817,14 @@
       <c t="n" r="U2">
         <v>1</v>
       </c>
-    </row>
-    <row spans="1:22" r="3">
+      <c t="s" r="V2">
+        <v>18</v>
+      </c>
+      <c t="n" r="W2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:24" r="3">
       <c t="s" r="F3">
         <v>12</v>
       </c>
@@ -859,8 +873,14 @@
       <c t="n" r="U3">
         <v>2</v>
       </c>
-    </row>
-    <row spans="1:22" r="4">
+      <c t="s" r="V3">
+        <v>16</v>
+      </c>
+      <c t="n" r="W3">
+        <v>2</v>
+      </c>
+    </row>
+    <row spans="1:24" r="4">
       <c t="s" r="I4">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Refactored export to excel so that padding is adjusted just at the end
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -41,7 +41,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>2;3</t>
+  </si>
+  <si>
+    <t>2;4</t>
+  </si>
   <si>
     <t>A</t>
   </si>
@@ -451,7 +457,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,25 +473,25 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>21</v>
-      </c>
-      <c t="n" r="B1">
-        <v>2.3</v>
-      </c>
-      <c t="n" r="C1">
-        <v>2.4</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="B1">
+        <v>0</v>
+      </c>
+      <c t="s" r="C1">
+        <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
@@ -522,25 +528,25 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>21</v>
-      </c>
-      <c t="n" r="B1">
-        <v>2.3</v>
-      </c>
-      <c t="n" r="C1">
-        <v>2.4</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="B1">
+        <v>0</v>
+      </c>
+      <c t="s" r="C1">
+        <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
@@ -548,7 +554,7 @@
         <v>0</v>
       </c>
       <c t="s" r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row spans="1:3" r="3">
@@ -556,7 +562,7 @@
         <v>1</v>
       </c>
       <c t="s" r="C3">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -571,25 +577,25 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>21</v>
-      </c>
-      <c t="n" r="B1">
-        <v>2.3</v>
-      </c>
-      <c t="n" r="C1">
-        <v>2.4</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="B1">
+        <v>0</v>
+      </c>
+      <c t="s" r="C1">
+        <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
@@ -626,25 +632,25 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="9.1"/>
-    <col customWidth="true" max="3" min="3" width="9.1"/>
-    <col customWidth="true" max="2" min="2" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
       <c t="s" r="A1">
-        <v>21</v>
-      </c>
-      <c t="n" r="B1">
-        <v>2.3</v>
-      </c>
-      <c t="n" r="C1">
-        <v>2.4</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="B1">
+        <v>0</v>
+      </c>
+      <c t="s" r="C1">
+        <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
@@ -652,7 +658,7 @@
         <v>0</v>
       </c>
       <c t="s" r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row spans="1:3" r="3">
@@ -660,7 +666,7 @@
         <v>1</v>
       </c>
       <c t="s" r="C3">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -675,79 +681,79 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col max="12" min="12" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
     <col max="24" min="24" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
+    <col max="23" min="23" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
     <col max="17" min="17" width="9.10"/>
-    <col max="16" min="16" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
     <col max="19" min="19" width="9.10"/>
-    <col max="18" min="18" width="9.10"/>
-    <col max="21" min="21" width="9.10"/>
-    <col max="20" min="20" width="9.10"/>
-    <col max="23" min="23" width="9.10"/>
-    <col max="22" min="22" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="15" min="15" width="9.10"/>
-    <col max="14" min="14" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
   </cols>
   <sheetData>
     <row spans="1:24" r="1">
       <c t="s" r="A1">
+        <v>11</v>
+      </c>
+      <c t="s" r="B1">
+        <v>24</v>
+      </c>
+      <c t="s" r="C1">
+        <v>11</v>
+      </c>
+      <c t="s" r="D1">
+        <v>14</v>
+      </c>
+      <c t="s" r="E1">
+        <v>5</v>
+      </c>
+      <c t="s" r="F1">
+        <v>11</v>
+      </c>
+      <c t="s" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" r="I1">
+        <v>8</v>
+      </c>
+      <c t="s" r="K1">
         <v>9</v>
       </c>
-      <c t="s" r="B1">
+      <c t="s" r="N1">
+        <v>10</v>
+      </c>
+      <c t="s" r="P1">
+        <v>17</v>
+      </c>
+      <c t="s" r="R1">
+        <v>21</v>
+      </c>
+      <c t="s" r="T1">
         <v>22</v>
       </c>
-      <c t="s" r="C1">
-        <v>9</v>
-      </c>
-      <c t="s" r="D1">
-        <v>12</v>
-      </c>
-      <c t="s" r="E1">
-        <v>3</v>
-      </c>
-      <c t="s" r="F1">
-        <v>9</v>
-      </c>
-      <c t="s" r="G1">
-        <v>4</v>
-      </c>
-      <c t="s" r="I1">
-        <v>6</v>
-      </c>
-      <c t="s" r="K1">
-        <v>7</v>
-      </c>
-      <c t="s" r="N1">
-        <v>8</v>
-      </c>
-      <c t="s" r="P1">
-        <v>15</v>
-      </c>
-      <c t="s" r="R1">
-        <v>19</v>
-      </c>
-      <c t="s" r="T1">
-        <v>20</v>
-      </c>
       <c t="s" r="V1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c t="n" r="X1">
         <v>0</v>
@@ -755,70 +761,70 @@
     </row>
     <row spans="1:24" r="2">
       <c t="s" r="A2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="B2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c t="s" r="C2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c t="s" r="E2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c t="s" r="F2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="G2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="n" r="H2">
         <v>1</v>
       </c>
       <c t="s" r="I2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c t="n" r="J2">
         <v>0</v>
       </c>
       <c t="s" r="K2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="L2">
         <v>2</v>
       </c>
       <c t="s" r="M2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c t="s" r="N2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="n" r="O2">
         <v>1</v>
       </c>
       <c t="s" r="P2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="Q2">
         <v>2</v>
       </c>
       <c t="s" r="R2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="n" r="S2">
         <v>1</v>
       </c>
       <c t="s" r="T2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="n" r="U2">
         <v>1</v>
       </c>
       <c t="s" r="V2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="n" r="W2">
         <v>1</v>
@@ -826,55 +832,55 @@
     </row>
     <row spans="1:24" r="3">
       <c t="s" r="F3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="G3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="H3">
         <v>2</v>
       </c>
       <c t="s" r="I3">
+        <v>20</v>
+      </c>
+      <c t="n" r="J3">
+        <v>1</v>
+      </c>
+      <c t="s" r="K3">
+        <v>20</v>
+      </c>
+      <c t="n" r="L3">
+        <v>1</v>
+      </c>
+      <c t="s" r="M3">
+        <v>3</v>
+      </c>
+      <c t="s" r="N3">
         <v>18</v>
-      </c>
-      <c t="n" r="J3">
-        <v>1</v>
-      </c>
-      <c t="s" r="K3">
-        <v>18</v>
-      </c>
-      <c t="n" r="L3">
-        <v>1</v>
-      </c>
-      <c t="s" r="M3">
-        <v>1</v>
-      </c>
-      <c t="s" r="N3">
-        <v>16</v>
       </c>
       <c t="n" r="O3">
         <v>2</v>
       </c>
       <c t="s" r="P3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="n" r="Q3">
         <v>1</v>
       </c>
       <c t="s" r="R3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="S3">
         <v>2</v>
       </c>
       <c t="s" r="T3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="U3">
         <v>2</v>
       </c>
       <c t="s" r="V3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="W3">
         <v>2</v>
@@ -882,22 +888,22 @@
     </row>
     <row spans="1:24" r="4">
       <c t="s" r="I4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="J4">
         <v>2</v>
       </c>
       <c t="s" r="K4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="n" r="L4">
         <v>2</v>
       </c>
       <c t="s" r="M4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="N4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c t="n" r="O4">
         <v>4</v>

</xml_diff>

<commit_message>
Changed where it checks that all row and column headers are the same length
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -452,7 +452,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
@@ -468,7 +468,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -478,41 +478,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col max="2" min="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" width="9.1" customWidth="true"/>
+    <col max="1" min="1" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="n" r="B3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -523,7 +523,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -533,35 +533,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col max="2" min="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" width="9.1" customWidth="true"/>
+    <col max="1" min="1" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="s" r="C3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -572,7 +572,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -582,41 +582,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col max="2" min="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" width="9.1" customWidth="true"/>
+    <col max="1" min="1" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="n" r="B3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -627,7 +627,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -637,35 +637,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" customWidth="true" min="1" width="9.1"/>
-    <col max="2" customWidth="true" min="2" width="9.1"/>
-    <col max="3" customWidth="true" min="3" width="9.1"/>
+    <col max="2" min="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" width="9.1" customWidth="true"/>
+    <col max="1" min="1" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
-        <v>1</v>
-      </c>
-      <c t="s" r="C3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -676,7 +676,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
@@ -686,226 +686,226 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="12" min="12" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="14" min="14" width="9.10"/>
-    <col max="15" min="15" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="7" min="7" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="24" min="24" width="9.10"/>
-    <col max="20" min="20" width="9.10"/>
-    <col max="21" min="21" width="9.10"/>
-    <col max="22" min="22" width="9.10"/>
-    <col max="23" min="23" width="9.10"/>
-    <col max="16" min="16" width="9.10"/>
-    <col max="17" min="17" width="9.10"/>
-    <col max="18" min="18" width="9.10"/>
-    <col max="19" min="19" width="9.10"/>
+    <col min="6" width="9.10" max="6"/>
+    <col min="7" width="9.10" max="7"/>
+    <col min="4" width="9.10" max="4"/>
+    <col min="5" width="9.10" max="5"/>
+    <col min="2" width="9.10" max="2"/>
+    <col min="3" width="9.10" max="3"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="14" width="9.10" max="14"/>
+    <col min="15" width="9.10" max="15"/>
+    <col min="12" width="9.10" max="12"/>
+    <col min="13" width="9.10" max="13"/>
+    <col min="10" width="9.10" max="10"/>
+    <col min="11" width="9.10" max="11"/>
+    <col min="8" width="9.10" max="8"/>
+    <col min="9" width="9.10" max="9"/>
+    <col min="22" width="9.10" max="22"/>
+    <col min="23" width="9.10" max="23"/>
+    <col min="20" width="9.10" max="20"/>
+    <col min="21" width="9.10" max="21"/>
+    <col min="18" width="9.10" max="18"/>
+    <col min="19" width="9.10" max="19"/>
+    <col min="16" width="9.10" max="16"/>
+    <col min="17" width="9.10" max="17"/>
+    <col min="24" width="9.10" max="24"/>
   </cols>
   <sheetData>
-    <row spans="1:24" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="K1">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="N1">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="P1">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="R1">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="T1">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="V1">
+      <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="X1">
+      <c r="X1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:24" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="G2">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="H2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I2">
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="J2">
+      <c r="J2" t="n">
         <v>0</v>
       </c>
-      <c t="s" r="K2">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="L2">
+      <c r="L2" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="M2">
+      <c r="M2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="N2">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="O2">
-        <v>1</v>
-      </c>
-      <c t="s" r="P2">
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>4</v>
       </c>
-      <c t="n" r="Q2">
+      <c r="Q2" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="R2">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="S2">
-        <v>1</v>
-      </c>
-      <c t="s" r="T2">
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="U2">
-        <v>1</v>
-      </c>
-      <c t="s" r="V2">
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="W2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:24" r="3">
-      <c t="s" r="F3">
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="G3">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="H3">
+      <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="I3">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="J3">
-        <v>1</v>
-      </c>
-      <c t="s" r="K3">
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="L3">
-        <v>1</v>
-      </c>
-      <c t="s" r="M3">
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="N3">
+      <c r="N3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="O3">
+      <c r="O3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="P3">
+      <c r="P3" t="s">
         <v>2</v>
       </c>
-      <c t="n" r="Q3">
-        <v>1</v>
-      </c>
-      <c t="s" r="R3">
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="S3">
+      <c r="S3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="T3">
+      <c r="T3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="U3">
+      <c r="U3" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="V3">
+      <c r="V3" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="W3">
+      <c r="W3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:24" r="4">
-      <c t="s" r="I4">
+    <row r="4" spans="1:24">
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="J4">
+      <c r="J4" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="K4">
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="L4">
+      <c r="L4" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="M4">
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="N4">
+      <c r="N4" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="O4">
+      <c r="O4" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Blank demographic includes blank menu
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -478,9 +478,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="2" min="2" width="9.1" customWidth="true"/>
-    <col max="3" min="3" width="9.1" customWidth="true"/>
-    <col max="1" min="1" width="9.1" customWidth="true"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -533,9 +533,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="2" min="2" width="9.1" customWidth="true"/>
-    <col max="3" min="3" width="9.1" customWidth="true"/>
-    <col max="1" min="1" width="9.1" customWidth="true"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -582,9 +582,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="2" min="2" width="9.1" customWidth="true"/>
-    <col max="3" min="3" width="9.1" customWidth="true"/>
-    <col max="1" min="1" width="9.1" customWidth="true"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -637,9 +637,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="2" min="2" width="9.1" customWidth="true"/>
-    <col max="3" min="3" width="9.1" customWidth="true"/>
-    <col max="1" min="1" width="9.1" customWidth="true"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Create default order for menu
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -27,9 +27,11 @@
     <definedName name="hist_sig_value_col_head">'HistSignificanceValues'!$B$1:$C$1</definedName>
     <definedName name="hist_sig_value_row_head">'HistSignificanceValues'!$A$2:$A$3</definedName>
     <definedName name="hist_sig_value_values">'HistSignificanceValues'!$B$2:$C$3</definedName>
-    <definedName name="cuts_config">'Lookups'!$A$1:$E$2</definedName>
-    <definedName name="cuts">'Lookups'!$F$1:$F$2</definedName>
-    <definedName name="cuts_historical">'Lookups'!$F$3:$F$3</definedName>
+    <definedName name="cuts_config">'Lookups'!$A$1:$E$3</definedName>
+    <definedName name="cuts">'Lookups'!$F$1:$F$3</definedName>
+    <definedName name="cuts_historical">'Lookups'!$F$4:$F$4</definedName>
+    <definedName name="cuts_2">'Lookups'!$F$5:$F$4</definedName>
+    <definedName name="cuts_3">'Lookups'!$F$5:$F$4</definedName>
     <definedName name="default_menu">'Lookups'!$F$2:$F$101</definedName>
     <definedName name="default_mapping">'Lookups'!$F$2:$G$101</definedName>
     <definedName name="default_menu_start">'Lookups'!$F$2</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>2;3</t>
   </si>
@@ -83,6 +85,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>Region</t>
@@ -450,14 +455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,26 +471,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -521,26 +526,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -562,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -570,26 +575,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -625,26 +630,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" width="9.1" customWidth="true" max="2"/>
-    <col min="3" width="9.1" customWidth="true" max="3"/>
-    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -666,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -674,42 +679,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" width="9.10" max="6"/>
-    <col min="7" width="9.10" max="7"/>
-    <col min="4" width="9.10" max="4"/>
-    <col min="5" width="9.10" max="5"/>
-    <col min="2" width="9.10" max="2"/>
-    <col min="3" width="9.10" max="3"/>
-    <col min="1" width="9.10" max="1"/>
-    <col min="14" width="9.10" max="14"/>
-    <col min="15" width="9.10" max="15"/>
-    <col min="12" width="9.10" max="12"/>
-    <col min="13" width="9.10" max="13"/>
-    <col min="10" width="9.10" max="10"/>
-    <col min="11" width="9.10" max="11"/>
-    <col min="8" width="9.10" max="8"/>
-    <col min="9" width="9.10" max="9"/>
-    <col min="22" width="9.10" max="22"/>
-    <col min="23" width="9.10" max="23"/>
-    <col min="20" width="9.10" max="20"/>
-    <col min="21" width="9.10" max="21"/>
-    <col min="18" width="9.10" max="18"/>
-    <col min="19" width="9.10" max="19"/>
-    <col min="16" width="9.10" max="16"/>
-    <col min="17" width="9.10" max="17"/>
-    <col min="24" width="9.10" max="24"/>
+    <col max="24" min="24" width="9.10"/>
+    <col max="23" min="23" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="19" min="19" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
+    <col max="17" min="17" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -717,19 +722,19 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -744,16 +749,16 @@
         <v>10</v>
       </c>
       <c r="P1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X1" t="n">
         <v>0</v>
@@ -761,13 +766,13 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -776,10 +781,10 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -791,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="n">
         <v>2</v>
@@ -800,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O2" t="n">
         <v>1</v>
@@ -812,42 +817,57 @@
         <v>2</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U2" t="n">
         <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" t="n">
         <v>1</v>
@@ -856,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O3" t="n">
         <v>2</v>
@@ -868,42 +888,45 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S3" t="n">
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U3" t="n">
         <v>2</v>
       </c>
       <c r="V3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="W3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:24">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="n">
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Fixing bug in statistical significance where comparison population is the same as the target population
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -9,16 +9,41 @@
   <sheets>
     <sheet name="ExistingData" r:id="rId1" sheetId="1"/>
     <sheet name="DisplayValues" r:id="rId2" sheetId="2"/>
+    <sheet name="SignificanceValues" r:id="rId3" sheetId="3"/>
+    <sheet name="HistDisplayValues" r:id="rId4" sheetId="4"/>
+    <sheet name="HistSignificanceValues" r:id="rId5" sheetId="5"/>
+    <sheet name="Lookups" r:id="rId6" sheetId="6"/>
   </sheets>
   <definedNames>
-    <definedName name="disp_value_col_head">'ExistingData'!$A$1</definedName>
+    <definedName name="disp_value_col_head">'DisplayValues'!$B$1:$C$1</definedName>
+    <definedName name="disp_value_row_head">'DisplayValues'!$A$2:$A$3</definedName>
+    <definedName name="disp_value_values">'DisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="sig_value_col_head">'SignificanceValues'!$B$1:$C$1</definedName>
+    <definedName name="sig_value_row_head">'SignificanceValues'!$A$2:$A$3</definedName>
+    <definedName name="sig_value_values">'SignificanceValues'!$B$2:$C$3</definedName>
+    <definedName name="hist_disp_value_col_head">'HistDisplayValues'!$B$1:$C$1</definedName>
+    <definedName name="hist_disp_value_row_head">'HistDisplayValues'!$A$2:$A$3</definedName>
+    <definedName name="hist_disp_value_values">'HistDisplayValues'!$B$2:$C$3</definedName>
+    <definedName name="hist_sig_value_col_head">'HistSignificanceValues'!$B$1:$C$1</definedName>
+    <definedName name="hist_sig_value_row_head">'HistSignificanceValues'!$A$2:$A$3</definedName>
+    <definedName name="hist_sig_value_values">'HistSignificanceValues'!$B$2:$C$3</definedName>
+    <definedName name="cuts_config">'Lookups'!$A$1:$E$3</definedName>
+    <definedName name="cuts">'Lookups'!$F$1:$F$3</definedName>
+    <definedName name="cuts_historical">'Lookups'!$F$4:$F$4</definedName>
+    <definedName name="cuts_2">'Lookups'!$F$5:$F$4</definedName>
+    <definedName name="cuts_3">'Lookups'!$F$5:$F$4</definedName>
+    <definedName name="default_menu">'Lookups'!$F$2:$F$101</definedName>
+    <definedName name="default_mapping">'Lookups'!$F$2:$G$101</definedName>
+    <definedName name="default_menu_start">'Lookups'!$F$2</definedName>
+    <definedName name="cuts_head">'Lookups'!$G$1:$W$1</definedName>
+    <definedName name="zero_string">'Lookups'!$X$1</definedName>
   </definedNames>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>2;3</t>
   </si>
@@ -26,7 +51,79 @@
     <t>2;4</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Corps</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Gender Not Used</t>
+  </si>
+  <si>
+    <t>GenderB</t>
+  </si>
+  <si>
+    <t>GenderC</t>
+  </si>
+  <si>
+    <t>Gender_LIB</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SoDak</t>
+  </si>
+  <si>
+    <t>ValueOrderDimension</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>lib</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>question_code</t>
+  </si>
+  <si>
+    <t>result_type</t>
+  </si>
+  <si>
     <t>row_heading</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>survey_code</t>
   </si>
 </sst>
 </file>
@@ -386,14 +483,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="1" max="1"/>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -426,4 +523,415 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" width="9.1" min="2" max="2"/>
+    <col customWidth="true" width="9.1" min="3" max="3"/>
+    <col customWidth="true" width="9.1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col width="9.10" min="2" max="2"/>
+    <col width="9.10" min="3" max="3"/>
+    <col width="9.10" min="1" max="1"/>
+    <col width="9.10" min="6" max="6"/>
+    <col width="9.10" min="7" max="7"/>
+    <col width="9.10" min="4" max="4"/>
+    <col width="9.10" min="5" max="5"/>
+    <col width="9.10" min="10" max="10"/>
+    <col width="9.10" min="11" max="11"/>
+    <col width="9.10" min="8" max="8"/>
+    <col width="9.10" min="9" max="9"/>
+    <col width="9.10" min="14" max="14"/>
+    <col width="9.10" min="15" max="15"/>
+    <col width="9.10" min="12" max="12"/>
+    <col width="9.10" min="13" max="13"/>
+    <col width="9.10" min="18" max="18"/>
+    <col width="9.10" min="19" max="19"/>
+    <col width="9.10" min="16" max="16"/>
+    <col width="9.10" min="17" max="17"/>
+    <col width="9.10" min="22" max="22"/>
+    <col width="9.10" min="23" max="23"/>
+    <col width="9.10" min="20" max="20"/>
+    <col width="9.10" min="21" max="21"/>
+    <col width="9.10" min="24" max="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Attempt to reduce memory load between runs
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -462,7 +462,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -478,14 +478,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col min="1" max="1" width="9.1" customWidth="true"/>
+    <col min="3" max="3" width="9.1" customWidth="true"/>
+    <col min="2" max="2" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -533,14 +533,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col min="1" max="1" width="9.1" customWidth="true"/>
+    <col min="3" max="3" width="9.1" customWidth="true"/>
+    <col min="2" max="2" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -582,14 +582,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col min="1" max="1" width="9.1" customWidth="true"/>
+    <col min="3" max="3" width="9.1" customWidth="true"/>
+    <col min="2" max="2" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -637,14 +637,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" width="9.1" min="2" max="2"/>
-    <col customWidth="true" width="9.1" min="3" max="3"/>
-    <col customWidth="true" width="9.1" min="1" max="1"/>
+    <col min="1" max="1" width="9.1" customWidth="true"/>
+    <col min="3" max="3" width="9.1" customWidth="true"/>
+    <col min="2" max="2" width="9.1" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -686,35 +686,35 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
-    <col width="9.10" min="1" max="1"/>
-    <col width="9.10" min="6" max="6"/>
-    <col width="9.10" min="7" max="7"/>
-    <col width="9.10" min="4" max="4"/>
-    <col width="9.10" min="5" max="5"/>
-    <col width="9.10" min="10" max="10"/>
-    <col width="9.10" min="11" max="11"/>
-    <col width="9.10" min="8" max="8"/>
-    <col width="9.10" min="9" max="9"/>
-    <col width="9.10" min="14" max="14"/>
-    <col width="9.10" min="15" max="15"/>
-    <col width="9.10" min="12" max="12"/>
-    <col width="9.10" min="13" max="13"/>
-    <col width="9.10" min="18" max="18"/>
-    <col width="9.10" min="19" max="19"/>
-    <col width="9.10" min="16" max="16"/>
-    <col width="9.10" min="17" max="17"/>
-    <col width="9.10" min="22" max="22"/>
-    <col width="9.10" min="23" max="23"/>
-    <col width="9.10" min="20" max="20"/>
-    <col width="9.10" min="21" max="21"/>
-    <col width="9.10" min="24" max="24"/>
+    <col min="21" max="21" width="9.10"/>
+    <col min="20" max="20" width="9.10"/>
+    <col min="23" max="23" width="9.10"/>
+    <col min="22" max="22" width="9.10"/>
+    <col min="17" max="17" width="9.10"/>
+    <col min="16" max="16" width="9.10"/>
+    <col min="19" max="19" width="9.10"/>
+    <col min="18" max="18" width="9.10"/>
+    <col min="24" max="24" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="7" max="7" width="9.10"/>
+    <col min="6" max="6" width="9.10"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="13" max="13" width="9.10"/>
+    <col min="12" max="12" width="9.10"/>
+    <col min="15" max="15" width="9.10"/>
+    <col min="14" max="14" width="9.10"/>
+    <col min="9" max="9" width="9.10"/>
+    <col min="8" max="8" width="9.10"/>
+    <col min="11" max="11" width="9.10"/>
+    <col min="10" max="10" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">

</xml_diff>

<commit_message>
Slowly refactoring for flushing of calculations to keep memory down
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -462,7 +462,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -478,17 +478,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1" customWidth="true"/>
-    <col min="3" max="3" width="9.1" customWidth="true"/>
-    <col min="2" max="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row spans="1:3" r="1">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row spans="1:3" r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
@@ -510,7 +510,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row spans="1:3" r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
@@ -533,17 +533,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1" customWidth="true"/>
-    <col min="3" max="3" width="9.1" customWidth="true"/>
-    <col min="2" max="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row spans="1:3" r="1">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row spans="1:3" r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
@@ -562,7 +562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row spans="1:3" r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
@@ -582,17 +582,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1" customWidth="true"/>
-    <col min="3" max="3" width="9.1" customWidth="true"/>
-    <col min="2" max="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row spans="1:3" r="1">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row spans="1:3" r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
@@ -614,7 +614,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row spans="1:3" r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
@@ -637,17 +637,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1" customWidth="true"/>
-    <col min="3" max="3" width="9.1" customWidth="true"/>
-    <col min="2" max="2" width="9.1" customWidth="true"/>
+    <col max="3" min="3" customWidth="true" width="9.1"/>
+    <col max="2" min="2" customWidth="true" width="9.1"/>
+    <col max="1" min="1" customWidth="true" width="9.1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row spans="1:3" r="1">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row spans="1:3" r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
@@ -666,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row spans="1:3" r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
@@ -686,38 +686,38 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="21" max="21" width="9.10"/>
-    <col min="20" max="20" width="9.10"/>
-    <col min="23" max="23" width="9.10"/>
-    <col min="22" max="22" width="9.10"/>
-    <col min="17" max="17" width="9.10"/>
-    <col min="16" max="16" width="9.10"/>
-    <col min="19" max="19" width="9.10"/>
-    <col min="18" max="18" width="9.10"/>
-    <col min="24" max="24" width="9.10"/>
-    <col min="5" max="5" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
-    <col min="7" max="7" width="9.10"/>
-    <col min="6" max="6" width="9.10"/>
-    <col min="1" max="1" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
-    <col min="13" max="13" width="9.10"/>
-    <col min="12" max="12" width="9.10"/>
-    <col min="15" max="15" width="9.10"/>
-    <col min="14" max="14" width="9.10"/>
-    <col min="9" max="9" width="9.10"/>
-    <col min="8" max="8" width="9.10"/>
-    <col min="11" max="11" width="9.10"/>
-    <col min="10" max="10" width="9.10"/>
+    <col max="23" min="23" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="19" min="19" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
+    <col max="17" min="17" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
+    <col max="24" min="24" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row spans="1:24" r="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row spans="1:24" r="2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -835,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row spans="1:24" r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -906,7 +906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row spans="1:24" r="4">
       <c r="F4" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
More refactoring - will this work?
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -483,41 +483,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="3" customWidth="true" width="9.1"/>
-    <col max="2" min="2" customWidth="true" width="9.1"/>
-    <col max="1" min="1" customWidth="true" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -538,35 +538,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="3" customWidth="true" width="9.1"/>
-    <col max="2" min="2" customWidth="true" width="9.1"/>
-    <col max="1" min="1" customWidth="true" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>12</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
         <v>16</v>
       </c>
     </row>
@@ -587,41 +587,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="3" customWidth="true" width="9.1"/>
-    <col max="2" min="2" customWidth="true" width="9.1"/>
-    <col max="1" min="1" customWidth="true" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>0.5</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="n" r="B3">
         <v>0.5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>0.5</v>
       </c>
     </row>
@@ -642,35 +642,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="3" customWidth="true" width="9.1"/>
-    <col max="2" min="2" customWidth="true" width="9.1"/>
-    <col max="1" min="1" customWidth="true" width="9.1"/>
+    <col max="1" customWidth="true" min="1" width="9.1"/>
+    <col max="2" customWidth="true" min="2" width="9.1"/>
+    <col max="3" customWidth="true" min="3" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:3" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>1</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="A2" t="n">
+      <c t="n" r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>12</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c t="n" r="A3">
+        <v>1</v>
+      </c>
+      <c t="s" r="C3">
         <v>16</v>
       </c>
     </row>
@@ -691,244 +691,244 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col max="24" min="24" width="9.10"/>
+    <col max="16" min="16" width="9.10"/>
+    <col max="17" min="17" width="9.10"/>
+    <col max="18" min="18" width="9.10"/>
+    <col max="19" min="19" width="9.10"/>
+    <col max="20" min="20" width="9.10"/>
+    <col max="21" min="21" width="9.10"/>
+    <col max="22" min="22" width="9.10"/>
     <col max="23" min="23" width="9.10"/>
-    <col max="22" min="22" width="9.10"/>
-    <col max="21" min="21" width="9.10"/>
-    <col max="20" min="20" width="9.10"/>
-    <col max="19" min="19" width="9.10"/>
-    <col max="18" min="18" width="9.10"/>
-    <col max="17" min="17" width="9.10"/>
-    <col max="16" min="16" width="9.10"/>
-    <col max="24" min="24" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
+    <col max="10" min="10" width="9.10"/>
+    <col max="11" min="11" width="9.10"/>
+    <col max="12" min="12" width="9.10"/>
+    <col max="13" min="13" width="9.10"/>
+    <col max="14" min="14" width="9.10"/>
+    <col max="15" min="15" width="9.10"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
     <col max="7" min="7" width="9.10"/>
-    <col max="6" min="6" width="9.10"/>
-    <col max="5" min="5" width="9.10"/>
-    <col max="4" min="4" width="9.10"/>
-    <col max="3" min="3" width="9.10"/>
-    <col max="2" min="2" width="9.10"/>
-    <col max="1" min="1" width="9.10"/>
-    <col max="15" min="15" width="9.10"/>
-    <col max="14" min="14" width="9.10"/>
-    <col max="13" min="13" width="9.10"/>
-    <col max="12" min="12" width="9.10"/>
-    <col max="11" min="11" width="9.10"/>
-    <col max="10" min="10" width="9.10"/>
-    <col max="9" min="9" width="9.10"/>
-    <col max="8" min="8" width="9.10"/>
   </cols>
   <sheetData>
     <row spans="1:24" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c t="s" r="B1">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c t="s" r="C1">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c t="s" r="D1">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c t="s" r="E1">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c t="s" r="F1">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c t="s" r="G1">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c t="s" r="I1">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c t="s" r="K1">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c t="s" r="N1">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c t="s" r="P1">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c t="s" r="R1">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c t="s" r="T1">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c t="s" r="V1">
         <v>26</v>
       </c>
-      <c r="X1" t="n">
+      <c t="n" r="X1">
         <v>0</v>
       </c>
     </row>
     <row spans="1:24" r="2">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c t="s" r="C2">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c t="s" r="D2">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c t="s" r="E2">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c t="s" r="F2">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c t="s" r="G2">
         <v>21</v>
       </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c t="n" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I2">
         <v>7</v>
       </c>
-      <c r="J2" t="n">
+      <c t="n" r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c t="s" r="K2">
         <v>19</v>
       </c>
-      <c r="L2" t="n">
+      <c t="n" r="L2">
         <v>2</v>
       </c>
-      <c r="M2" t="s">
+      <c t="s" r="M2">
         <v>3</v>
       </c>
-      <c r="N2" t="s">
+      <c t="s" r="N2">
         <v>21</v>
       </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+      <c t="n" r="O2">
+        <v>1</v>
+      </c>
+      <c t="s" r="P2">
         <v>4</v>
       </c>
-      <c r="Q2" t="n">
+      <c t="n" r="Q2">
         <v>2</v>
       </c>
-      <c r="R2" t="s">
+      <c t="s" r="R2">
         <v>21</v>
       </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c t="n" r="S2">
+        <v>1</v>
+      </c>
+      <c t="s" r="T2">
         <v>21</v>
       </c>
-      <c r="U2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
+      <c t="n" r="U2">
+        <v>1</v>
+      </c>
+      <c t="s" r="V2">
         <v>21</v>
       </c>
-      <c r="W2" t="n">
+      <c t="n" r="W2">
         <v>1</v>
       </c>
     </row>
     <row spans="1:24" r="3">
-      <c r="A3" t="s">
+      <c t="s" r="A3">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c t="s" r="C3">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c t="s" r="D3">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c t="s" r="E3">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c t="s" r="F3">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c t="s" r="G3">
         <v>19</v>
       </c>
-      <c r="H3" t="n">
+      <c t="n" r="H3">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c t="s" r="I3">
         <v>21</v>
       </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c t="n" r="J3">
+        <v>1</v>
+      </c>
+      <c t="s" r="K3">
         <v>21</v>
       </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
+      <c t="n" r="L3">
+        <v>1</v>
+      </c>
+      <c t="s" r="M3">
         <v>3</v>
       </c>
-      <c r="N3" t="s">
+      <c t="s" r="N3">
         <v>19</v>
       </c>
-      <c r="O3" t="n">
+      <c t="n" r="O3">
         <v>2</v>
       </c>
-      <c r="P3" t="s">
+      <c t="s" r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c t="n" r="Q3">
+        <v>1</v>
+      </c>
+      <c t="s" r="R3">
         <v>19</v>
       </c>
-      <c r="S3" t="n">
+      <c t="n" r="S3">
         <v>2</v>
       </c>
-      <c r="T3" t="s">
+      <c t="s" r="T3">
         <v>19</v>
       </c>
-      <c r="U3" t="n">
+      <c t="n" r="U3">
         <v>2</v>
       </c>
-      <c r="V3" t="s">
+      <c t="s" r="V3">
         <v>19</v>
       </c>
-      <c r="W3" t="n">
+      <c t="n" r="W3">
         <v>2</v>
       </c>
     </row>
     <row spans="1:24" r="4">
-      <c r="F4" t="s">
+      <c t="s" r="F4">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c t="s" r="I4">
         <v>19</v>
       </c>
-      <c r="J4" t="n">
+      <c t="n" r="J4">
         <v>2</v>
       </c>
-      <c r="K4" t="s">
+      <c t="s" r="K4">
         <v>19</v>
       </c>
-      <c r="L4" t="n">
+      <c t="n" r="L4">
         <v>2</v>
       </c>
-      <c r="M4" t="s">
+      <c t="s" r="M4">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c t="s" r="N4">
         <v>20</v>
       </c>
-      <c r="O4" t="n">
+      <c t="n" r="O4">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a cuts_ menus labeling bug
</commit_message>
<xml_diff>
--- a/CalculationCoordinator/test_file.xlsx
+++ b/CalculationCoordinator/test_file.xlsx
@@ -30,10 +30,10 @@
     <s:definedName name="cuts_config">'Lookups'!$A$1:$E$3</s:definedName>
     <s:definedName name="cuts">'Lookups'!$F$1:$F$3</s:definedName>
     <s:definedName name="cuts_historical">'Lookups'!$F$4:$F$4</s:definedName>
-    <s:definedName name="cuts_2">'Lookups'!$F$5:$F$4</s:definedName>
-    <s:definedName name="cuts_3">'Lookups'!$F$5:$F$4</s:definedName>
-    <s:definedName name="cuts_4">'Lookups'!$F$5:$F$4</s:definedName>
-    <s:definedName name="cuts_5">'Lookups'!$F$5:$F$4</s:definedName>
+    <s:definedName name="cuts_2">'Lookups'!$F$5:$F$5</s:definedName>
+    <s:definedName name="cuts_3">'Lookups'!$F$6:$F$5</s:definedName>
+    <s:definedName name="cuts_4">'Lookups'!$F$6:$F$5</s:definedName>
+    <s:definedName name="cuts_5">'Lookups'!$F$6:$F$5</s:definedName>
     <s:definedName name="default_menu">'Lookups'!$F$2:$F$1001</s:definedName>
     <s:definedName name="default_mapping">'Lookups'!$F$2:$G$1001</s:definedName>
     <s:definedName name="default_menu_start">'Lookups'!$F$2</s:definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>row_heading</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>S</t>
@@ -174,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -471,15 +468,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
 </worksheet>
 </file>
@@ -487,46 +484,46 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c t="s" r="A1">
+    <row spans="1:3" r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c t="n" r="A2">
-        <v>0.0</v>
-      </c>
-      <c t="n" r="B2">
+    <row spans="1:3" r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c t="n" r="A3">
-        <v>1.0</v>
-      </c>
-      <c t="n" r="B3">
+    <row spans="1:3" r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -537,47 +534,43 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c t="s" r="A1">
+    <row spans="1:3" r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c t="n" r="A2">
-        <v>0.0</v>
-      </c>
-      <c t="s" r="B2">
+    <row spans="1:3" r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s"/>
+    </row>
+    <row spans="1:3" r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c t="n" r="A3">
-        <v>1.0</v>
-      </c>
-      <c t="s" r="B3">
-        <v>4</v>
-      </c>
-      <c t="s" r="C3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -587,46 +580,46 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c t="s" r="A1">
+    <row spans="1:3" r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c t="n" r="A2">
-        <v>0.0</v>
-      </c>
-      <c t="n" r="B2">
+    <row spans="1:3" r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c t="n" r="A3">
-        <v>1.0</v>
-      </c>
-      <c t="n" r="B3">
+    <row spans="1:3" r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -637,47 +630,43 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c t="s" r="A1">
+    <row spans="1:3" r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c t="n" r="A2">
-        <v>0.0</v>
-      </c>
-      <c t="s" r="B2">
+    <row spans="1:3" r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s"/>
+    </row>
+    <row spans="1:3" r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c t="n" r="A3">
-        <v>1.0</v>
-      </c>
-      <c t="s" r="B3">
-        <v>4</v>
-      </c>
-      <c t="s" r="C3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -687,231 +676,234 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c t="s" r="A1">
+    <row spans="1:24" r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="B1">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="C1">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row spans="1:24" r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="D1">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row spans="1:24" r="3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="F1">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="G1">
-        <v>10</v>
-      </c>
-      <c t="s" r="I1">
-        <v>11</v>
-      </c>
-      <c t="s" r="K1">
-        <v>12</v>
-      </c>
-      <c t="s" r="N1">
-        <v>13</v>
-      </c>
-      <c t="s" r="P1">
-        <v>14</v>
-      </c>
-      <c t="s" r="R1">
-        <v>15</v>
-      </c>
-      <c t="s" r="T1">
-        <v>16</v>
-      </c>
-      <c t="s" r="V1">
-        <v>17</v>
-      </c>
-      <c t="s" r="X1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c t="s" r="A2">
-        <v>8</v>
-      </c>
-      <c t="s" r="B2">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row spans="1:24" r="4">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="C2">
-        <v>8</v>
-      </c>
-      <c t="s" r="D2">
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row spans="1:24" r="5">
+      <c r="F5" t="s">
         <v>9</v>
-      </c>
-      <c t="s" r="E2">
-        <v>19</v>
-      </c>
-      <c t="s" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" r="G2">
-        <v>20</v>
-      </c>
-      <c t="s" r="H2">
-        <v>21</v>
-      </c>
-      <c t="s" r="I2">
-        <v>22</v>
-      </c>
-      <c t="s" r="J2">
-        <v>18</v>
-      </c>
-      <c t="s" r="K2">
-        <v>23</v>
-      </c>
-      <c t="s" r="L2">
-        <v>24</v>
-      </c>
-      <c t="s" r="M2">
-        <v>25</v>
-      </c>
-      <c t="s" r="N2">
-        <v>20</v>
-      </c>
-      <c t="s" r="O2">
-        <v>21</v>
-      </c>
-      <c t="s" r="P2">
-        <v>26</v>
-      </c>
-      <c t="s" r="Q2">
-        <v>24</v>
-      </c>
-      <c t="s" r="R2">
-        <v>20</v>
-      </c>
-      <c t="s" r="S2">
-        <v>21</v>
-      </c>
-      <c t="s" r="T2">
-        <v>20</v>
-      </c>
-      <c t="s" r="U2">
-        <v>21</v>
-      </c>
-      <c t="s" r="V2">
-        <v>20</v>
-      </c>
-      <c t="s" r="W2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c t="s" r="A3">
-        <v>10</v>
-      </c>
-      <c t="s" r="B3">
-        <v>7</v>
-      </c>
-      <c t="s" r="C3">
-        <v>10</v>
-      </c>
-      <c t="s" r="D3">
-        <v>8</v>
-      </c>
-      <c t="s" r="E3">
-        <v>9</v>
-      </c>
-      <c t="s" r="F3">
-        <v>10</v>
-      </c>
-      <c t="s" r="G3">
-        <v>23</v>
-      </c>
-      <c t="s" r="H3">
-        <v>24</v>
-      </c>
-      <c t="s" r="I3">
-        <v>20</v>
-      </c>
-      <c t="s" r="J3">
-        <v>21</v>
-      </c>
-      <c t="s" r="K3">
-        <v>20</v>
-      </c>
-      <c t="s" r="L3">
-        <v>21</v>
-      </c>
-      <c t="s" r="M3">
-        <v>25</v>
-      </c>
-      <c t="s" r="N3">
-        <v>23</v>
-      </c>
-      <c t="s" r="O3">
-        <v>24</v>
-      </c>
-      <c t="s" r="P3">
-        <v>27</v>
-      </c>
-      <c t="s" r="Q3">
-        <v>21</v>
-      </c>
-      <c t="s" r="R3">
-        <v>23</v>
-      </c>
-      <c t="s" r="S3">
-        <v>24</v>
-      </c>
-      <c t="s" r="T3">
-        <v>23</v>
-      </c>
-      <c t="s" r="U3">
-        <v>24</v>
-      </c>
-      <c t="s" r="V3">
-        <v>23</v>
-      </c>
-      <c t="s" r="W3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c t="s" r="I4">
-        <v>23</v>
-      </c>
-      <c t="s" r="J4">
-        <v>24</v>
-      </c>
-      <c t="s" r="K4">
-        <v>23</v>
-      </c>
-      <c t="s" r="L4">
-        <v>24</v>
-      </c>
-      <c t="s" r="M4">
-        <v>28</v>
-      </c>
-      <c t="s" r="N4">
-        <v>29</v>
-      </c>
-      <c t="s" r="O4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c t="s" r="F5">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>